<commit_message>
First phase of text analysis complete Formatted Category
</commit_message>
<xml_diff>
--- a/trial.xlsx
+++ b/trial.xlsx
@@ -1,15 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="before" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="cleaned" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Cleaned_FULL" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="before" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="cleaned" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cleaned_FULL" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="services" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="technologies" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sectors" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18875,4 +18878,1319 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Formatted services</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>sme support</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>technological innovation</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>knowledge transfer</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ecosystem building</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>technology transfer</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>innovation management</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>prototyping</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>sme business development</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>public sector innovation</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>finance</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>regional development</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>circular economy</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>vocational training</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>smart specialisation strategies</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>field trial</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Formatted technologies</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>artificial intelligence &amp; decision support</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>internet of things</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>cybersecurity</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>big data</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>digital twins</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>robotics</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>virtual reality</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>high performance computing</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>sensors &amp; vision processing systems</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>simulation engineering and modelling</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>additive manufacturing</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>cloud services</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>cyber-physical systems</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>internet services &amp; applications</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>communication network</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>blockchain and distributed ledger technology (dlt)</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>human computer interaction</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>mobility</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>software architectures</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>logistics</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>location-based applications</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>laser-based manufacturing and materials processing</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>gamification</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>quantum technologies (computing/communication)</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>optoelectronics</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>micro- and nanoelectronics</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>semiconductors and nanotechnology</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>new technologies for audio-visual sector - media</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>industrial biotechnology</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>bi tools</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>photonics</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>products)</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>chemical engineering (plants</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>displays</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>organic and large area electronics</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>data</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Formatted sectors</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>count</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>manufacturing and processing</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>energy</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>health care</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>smart city</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>public administration</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>education</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>environment</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>transport &amp; mobility</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>automotive</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>agricultural biotechnology and food biotechnology</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>construction &amp; assembly</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>metal working and industrial production</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>travel and tourism</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>telecommunications</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>food and beverages</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>life sciences</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>security</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>cultural and creative economy</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>retail</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>wholesale or distribution</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>financial</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>community-led local development</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>textiles</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>transport sector</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>consumer products</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>personal services</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>maritime</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>defence</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>polymers and plastics</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>aeronautics</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>space</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>electricity</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>nmp non-metallic materials &amp; basic processes</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>paper and wood</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>fuels and petroleum engineering</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>real estate</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>legal aspects</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>regulation</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>fishery</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>mining and extraction</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>leather</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>nuclear</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>tobacco</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates on web scrapping
</commit_message>
<xml_diff>
--- a/trial.xlsx
+++ b/trial.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="before" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="cleaned" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Cleaned_FULL" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="services" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="technologies" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="sectors" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="data required to be scrapped" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="missing info" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="before" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="cleaned" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Cleaned_FULL" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="services" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="technologies" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sectors" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="data required to be scrapped" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="missing info" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -836,7 +836,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -932,7 +932,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>Hungary</t>
         </is>
       </c>
       <c r="B10" t="n">
@@ -942,7 +942,7 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>Hungary</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -952,7 +952,7 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -972,7 +972,7 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>Türkiye</t>
+          <t>Belgium</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -982,7 +982,7 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>Belgium</t>
+          <t>Türkiye</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -1012,7 +1012,7 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>Serbia</t>
+          <t>Slovenia</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -1022,7 +1022,7 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>Croatia</t>
+          <t>Serbia</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -1032,7 +1032,7 @@
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>Slovenia</t>
+          <t>Denmark</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -1042,7 +1042,7 @@
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Slovakia</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -1052,7 +1052,7 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>Slovakia</t>
+          <t>Croatia</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -1062,7 +1062,7 @@
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>Ireland</t>
+          <t>Albania</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -1072,7 +1072,7 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>Albania</t>
+          <t>Austria</t>
         </is>
       </c>
       <c r="B24" t="n">
@@ -1082,7 +1082,7 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>Austria</t>
+          <t>Lithuania</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -1102,7 +1102,7 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>North Macedonia</t>
+          <t>Ireland</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -1112,7 +1112,7 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>Lithuania</t>
+          <t>North Macedonia</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -1122,7 +1122,7 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>Norway</t>
+          <t>Latvia</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -1132,7 +1132,7 @@
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>Latvia</t>
+          <t>Norway</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -1142,7 +1142,7 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>Bosnia and Herzegovina</t>
+          <t>Malta</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -1152,7 +1152,7 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>Liechtenstein</t>
+          <t>Cyprus</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -1162,7 +1162,7 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>Cyprus</t>
+          <t>Liechtenstein</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -1172,7 +1172,7 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>Malta</t>
+          <t>Bosnia and Herzegovina</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -1182,7 +1182,7 @@
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>Iceland</t>
+          <t>Montenegro</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1212,10 +1212,20 @@
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>Montenegro</t>
+          <t>Iceland</t>
         </is>
       </c>
       <c r="B38" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>Estonia</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1230,7 +1240,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K298"/>
+  <dimension ref="A1:K299"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1239,11 +1249,6 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>EDIH Name</t>
-        </is>
-      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
           <t>EDIH Title</t>
@@ -1296,10 +1301,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Mittelstand-Digital Zentrum Berlin</t>
-        </is>
+      <c r="A2" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -1349,10 +1352,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Mittelstand-Digital Zentrum Handwerk</t>
-        </is>
+      <c r="A3" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -1402,10 +1403,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>CICERO DIH</t>
-        </is>
+      <c r="A4" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -1455,10 +1454,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>Idele</t>
-        </is>
+      <c r="A5" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -1508,10 +1505,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>C-Hub</t>
-        </is>
+      <c r="A6" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -1565,10 +1560,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>Data2Sustain</t>
-        </is>
+      <c r="A7" s="1" t="n">
+        <v>5</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -1622,10 +1615,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>InnovTourism DIH</t>
-        </is>
+      <c r="A8" s="1" t="n">
+        <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -1676,10 +1667,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>AIR-Andalusia</t>
-        </is>
+      <c r="A9" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1733,10 +1722,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>NASK - PIB</t>
-        </is>
+      <c r="A10" s="1" t="n">
+        <v>8</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1790,10 +1777,8 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
-        <is>
-          <t>SCS</t>
-        </is>
+      <c r="A11" s="1" t="n">
+        <v>9</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1847,10 +1832,8 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
-        <is>
-          <t>CIH</t>
-        </is>
+      <c r="A12" s="1" t="n">
+        <v>10</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1904,10 +1887,8 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="inlineStr">
-        <is>
-          <t>EDIH CTU</t>
-        </is>
+      <c r="A13" s="1" t="n">
+        <v>11</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1961,10 +1942,8 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="inlineStr">
-        <is>
-          <t>DIH4Society</t>
-        </is>
+      <c r="A14" s="1" t="n">
+        <v>12</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -2020,10 +1999,8 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="inlineStr">
-        <is>
-          <t>DIHGIGAL</t>
-        </is>
+      <c r="A15" s="1" t="n">
+        <v>13</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -2077,10 +2054,8 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>DIHNAMIC</t>
-        </is>
+      <c r="A16" s="1" t="n">
+        <v>14</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -2134,10 +2109,8 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
-          <t>EDCASS</t>
-        </is>
+      <c r="A17" s="1" t="n">
+        <v>15</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -2191,10 +2164,8 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>EDIH L</t>
-        </is>
+      <c r="A18" s="1" t="n">
+        <v>16</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -2257,10 +2228,8 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="inlineStr">
-        <is>
-          <t>EDIH MADRID REGION</t>
-        </is>
+      <c r="A19" s="1" t="n">
+        <v>17</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -2310,10 +2279,8 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="inlineStr">
-        <is>
-          <t>EDIH Suedwestfalen</t>
-        </is>
+      <c r="A20" s="1" t="n">
+        <v>18</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -2363,10 +2330,8 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="inlineStr">
-        <is>
-          <t>EDIH VILNIUS</t>
-        </is>
+      <c r="A21" s="1" t="n">
+        <v>19</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -2421,10 +2386,8 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="inlineStr">
-        <is>
-          <t>EDIH-DIGIMAT</t>
-        </is>
+      <c r="A22" s="1" t="n">
+        <v>20</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -2478,10 +2441,8 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="inlineStr">
-        <is>
-          <t>EDIHDO</t>
-        </is>
+      <c r="A23" s="1" t="n">
+        <v>21</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -2535,10 +2496,8 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="inlineStr">
-        <is>
-          <t>EDIHLV</t>
-        </is>
+      <c r="A24" s="1" t="n">
+        <v>22</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -2592,10 +2551,8 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="inlineStr">
-        <is>
-          <t>EDOcobot</t>
-        </is>
+      <c r="A25" s="1" t="n">
+        <v>23</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -2645,10 +2602,8 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="inlineStr">
-        <is>
-          <t>Flanders AI EDIH</t>
-        </is>
+      <c r="A26" s="1" t="n">
+        <v>24</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -2708,10 +2663,8 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="inlineStr">
-        <is>
-          <t>EDIH Saarland</t>
-        </is>
+      <c r="A27" s="1" t="n">
+        <v>25</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -2765,10 +2718,8 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="inlineStr">
-        <is>
-          <t>MicroCyber</t>
-        </is>
+      <c r="A28" s="1" t="n">
+        <v>26</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -2825,10 +2776,8 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="inlineStr">
-        <is>
-          <t>PDIH</t>
-        </is>
+      <c r="A29" s="1" t="n">
+        <v>27</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -2878,10 +2827,8 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="inlineStr">
-        <is>
-          <t>POLYTRONICS</t>
-        </is>
+      <c r="A30" s="1" t="n">
+        <v>28</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -2935,16 +2882,14 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="inlineStr">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
         <is>
           <t>PRODUTECH DIH</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>PRODUTECH DIH</t>
-        </is>
-      </c>
       <c r="C31" t="inlineStr">
         <is>
           <t>As European Digital Innovation Hub, PRODUTECH DIH has the mission to promote the digitalisation of the manufacturing industry, through a consistent and coherent dual intervention directed to both production technologies and manufacturing sectors, leveraging the role that production technologies assume in the digital and green transformation of the several sectors of the manufacturing industry. Gathering a critical mass of unique capacities, infrastructures, competencies, capabilities and associated services, and having a solid relational capital with the ecosystem of stakeholders, a track record of European intervention and of corridors with other EDIHs, PRODUTECH DIH articulates, provides and makes available to the industry, and pertinent stakeholders, a coherent set of support services within the 4 main functions attributed to European Digital Innovation Hubs: Test before invest, Skills and training, Support to find investments and Dynamization of the innovation ecosystem and networking. PRODUTECH DIH is a consortium of 19 organizations, gathering the Portuguese cluster of production technologies for manufacturing, a science park/incubator, industry’s sector-oriented technology centers, research and technology organizations and higher education and vocational training organizations, with multiple locations across Portugal, acting as multipliers of digital capacities and as access points to the hub, to the European Network of DIHs, pertinent stakeholders, such as Enterprise Europe Network, and initiatives, and providing key support services, within the domains foreseen by the Digital Europe Programme, towards the digital and green transformation of the industry. PRODUTECH DIH delivers a solid unique value proposition: (1) consistent consortium towards the digital and green transformation of the industry, (2) European intervention capacity and ambition and (3) a strategic synergic intervention Local-Regional-National-European.</t>
@@ -2992,10 +2937,8 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="inlineStr">
-        <is>
-          <t>SRC-EDIH</t>
-        </is>
+      <c r="A32" s="1" t="n">
+        <v>30</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -3045,10 +2988,8 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="inlineStr">
-        <is>
-          <t>ShiftLabs</t>
-        </is>
+      <c r="A33" s="1" t="n">
+        <v>31</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -3102,10 +3043,8 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="inlineStr">
-        <is>
-          <t>TDIH</t>
-        </is>
+      <c r="A34" s="1" t="n">
+        <v>32</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -3160,10 +3099,8 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="inlineStr">
-        <is>
-          <t>UDD</t>
-        </is>
+      <c r="A35" s="1" t="n">
+        <v>33</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -3213,10 +3150,8 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="inlineStr">
-        <is>
-          <t>WalHub</t>
-        </is>
+      <c r="A36" s="1" t="n">
+        <v>34</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -3270,10 +3205,8 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="inlineStr">
-        <is>
-          <t>i4CAMHUB</t>
-        </is>
+      <c r="A37" s="1" t="n">
+        <v>35</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -3335,10 +3268,8 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="inlineStr">
-        <is>
-          <t>AI5production</t>
-        </is>
+      <c r="A38" s="1" t="n">
+        <v>36</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -3388,10 +3319,8 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="inlineStr">
-        <is>
-          <t>RCDS</t>
-        </is>
+      <c r="A39" s="1" t="n">
+        <v>37</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -3445,10 +3374,8 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="inlineStr">
-        <is>
-          <t>AM-EDIH</t>
-        </is>
+      <c r="A40" s="1" t="n">
+        <v>38</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -3498,16 +3425,14 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="inlineStr">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
         <is>
           <t>CONNECT5</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>CONNECT5</t>
-        </is>
-      </c>
       <c r="C41" t="inlineStr">
         <is>
           <t>CONNECT5 – DIH for Connectivity, CPS, IoT, Cloud/Edge and Data Analytics aims to create and operate a national and European reference DIH supporting the digital and green transformation of SMEs and public organizations. CONNECT5 is a collaborative network, in the form of a Consortium of 12 entities (RTO, polytechnic institutes, universities), with high level of expertise in digital technologies, state-of-the-art infrastructures and a deep nation-wide network of contacts (companies, business associations, public entities, etc.) bringing together their complementary expertise and assets, to create a unique value platform. CONNECT5’s will leverage on its capabilities based on Cyber-Physical Systems (CPS), Internet of Things (IoT), Communications networks (5G and 6G), infrastructures (Cloud and Edge Computing), Big Data platforms and analytical data processing, supported by Artificial Intelligence (AI), Cybersecurity and High-performance computing (HPC) when required, enabling the target entities to evaluate its impacts and the feasibility to their business before further investing in it. The services provided by CONNECT5 will be based on the definition of a digital transformation strategy identified in close cooperation with the user materialised on a strategic road map validated through the 4 main domains: i. Test before invest; ii. Skills and training; iii. Support to find investment; iv. Innovation ecosystem and networking. Included in the action plan is also the Digital Maturity Assessment, transformation proposal and acceleration with the DTA. CONNECT5 will provide a wide range of services that will enable any beneficiary to access the latest knowledge, expertise and technology with a special focus on the connectivity dimension for testing and experimenting digital innovation relevant to their activity, matching their needs with digital solutions already available or in an advanced phase of deployment. CONNECT5 expertise is reinforced by national projects like 5GO (focused on communication technologies), AUGMANITY (focused on I4.0) and CITYCATALYST (Focused on smart cities) among other activities (OASC, Gaia-X).</t>
@@ -3555,10 +3480,8 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="inlineStr">
-        <is>
-          <t>EDIH DIGIHUB</t>
-        </is>
+      <c r="A42" s="1" t="n">
+        <v>40</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -3612,10 +3535,8 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="inlineStr">
-        <is>
-          <t>RCDSI NCIZ</t>
-        </is>
+      <c r="A43" s="1" t="n">
+        <v>41</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -3665,10 +3586,8 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="inlineStr">
-        <is>
-          <t>ARTES 5.0</t>
-        </is>
+      <c r="A44" s="1" t="n">
+        <v>42</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -3718,10 +3637,8 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="1" t="inlineStr">
-        <is>
-          <t>EDIH-GE</t>
-        </is>
+      <c r="A45" s="1" t="n">
+        <v>43</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -3771,10 +3688,8 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="inlineStr">
-        <is>
-          <t>IP4FVG - EDIH</t>
-        </is>
+      <c r="A46" s="1" t="n">
+        <v>44</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -3828,10 +3743,8 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="inlineStr">
-        <is>
-          <t>L-DIH</t>
-        </is>
+      <c r="A47" s="1" t="n">
+        <v>45</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -3881,10 +3794,8 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="inlineStr">
-        <is>
-          <t>MIGHTY EDIH</t>
-        </is>
+      <c r="A48" s="1" t="n">
+        <v>46</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -3938,10 +3849,8 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="inlineStr">
-        <is>
-          <t>BDIH_EDIH</t>
-        </is>
+      <c r="A49" s="1" t="n">
+        <v>47</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -3995,10 +3904,8 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="inlineStr">
-        <is>
-          <t>BIREX plus plus</t>
-        </is>
+      <c r="A50" s="1" t="n">
+        <v>48</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
@@ -4049,10 +3956,8 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="1" t="inlineStr">
-        <is>
-          <t>BOOST Robotic EastNL</t>
-        </is>
+      <c r="A51" s="1" t="n">
+        <v>49</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
@@ -4106,10 +4011,8 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="1" t="inlineStr">
-        <is>
-          <t>CYBIAH</t>
-        </is>
+      <c r="A52" s="1" t="n">
+        <v>50</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
@@ -4169,10 +4072,8 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="1" t="inlineStr">
-        <is>
-          <t>EDIH4CP-1</t>
-        </is>
+      <c r="A53" s="1" t="n">
+        <v>51</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -4222,10 +4123,8 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="1" t="inlineStr">
-        <is>
-          <t>DI4 LITHUANIAN ID</t>
-        </is>
+      <c r="A54" s="1" t="n">
+        <v>52</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
@@ -4295,10 +4194,8 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="1" t="inlineStr">
-        <is>
-          <t>DIGI-SI</t>
-        </is>
+      <c r="A55" s="1" t="n">
+        <v>53</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
@@ -4355,10 +4252,8 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="1" t="inlineStr">
-        <is>
-          <t>DIGITALIS</t>
-        </is>
+      <c r="A56" s="1" t="n">
+        <v>54</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
@@ -4412,10 +4307,8 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="1" t="inlineStr">
-        <is>
-          <t>DIGIVEST</t>
-        </is>
+      <c r="A57" s="1" t="n">
+        <v>55</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
@@ -4469,10 +4362,8 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="1" t="inlineStr">
-        <is>
-          <t>MECH-E-DIH</t>
-        </is>
+      <c r="A58" s="1" t="n">
+        <v>56</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
@@ -4522,10 +4413,8 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="1" t="inlineStr">
-        <is>
-          <t>DIHCUBE</t>
-        </is>
+      <c r="A59" s="1" t="n">
+        <v>57</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
@@ -4579,10 +4468,8 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="1" t="inlineStr">
-        <is>
-          <t>CLOTEX-HUB</t>
-        </is>
+      <c r="A60" s="1" t="n">
+        <v>58</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
@@ -4639,10 +4526,8 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="1" t="inlineStr">
-        <is>
-          <t>EDICS</t>
-        </is>
+      <c r="A61" s="1" t="n">
+        <v>59</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
@@ -4696,10 +4581,8 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="inlineStr">
-        <is>
-          <t>EDIH-CONNECT</t>
-        </is>
+      <c r="A62" s="1" t="n">
+        <v>60</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
@@ -4753,10 +4636,8 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="1" t="inlineStr">
-        <is>
-          <t>EDIH-EBE</t>
-        </is>
+      <c r="A63" s="1" t="n">
+        <v>61</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
@@ -4818,10 +4699,8 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" s="1" t="inlineStr">
-        <is>
-          <t>ER2Digit</t>
-        </is>
+      <c r="A64" s="1" t="n">
+        <v>62</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
@@ -4882,10 +4761,8 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="1" t="inlineStr">
-        <is>
-          <t>AI and Gaming EDIH</t>
-        </is>
+      <c r="A65" s="1" t="n">
+        <v>63</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
@@ -4939,10 +4816,8 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="1" t="inlineStr">
-        <is>
-          <t>Nemonoor</t>
-        </is>
+      <c r="A66" s="1" t="n">
+        <v>64</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
@@ -5006,16 +4881,14 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="1" t="inlineStr">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="inlineStr">
         <is>
           <t>nZEB Smart Home DIH</t>
         </is>
       </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>nZEB Smart Home DIH</t>
-        </is>
-      </c>
       <c r="C67" t="inlineStr">
         <is>
           <t>The nZEB Smart Home DIH, coordinated by CERTH's Information Technologies Institute (ITI), was established in early 2017 as the first Hub in Central Macedonia, and has been fully operational ever since. The nZEB Smart Home DIH is an active liaison between research and the markets, acting as a driving force for empowering market-oriented stakeholders with innovative digital solutions. The Smart Home’s technological orientation goes over multiple vertical domains, with special focus on Robotics (commercial or prototype units available for use, integration with devices and sensors, advanced manipulation and control features added), Artificial Intelligence (e.g. intuitive perception and cognition for robotic systems), Cyber physical systems (e.g. embedded systems), Internet of Things (e.g. connected devices, sensors and actuators networks), Simulation and modelling, Big Data, Blockchain, Visual Analytics, and more. One of the unique merits of the DIH is the actual nZEB Smart Home infrastructure. It is a unique Building based on state-of-the-art construction materials (insulation, glass panes, etc.) with "smart" technologies that allow the exploration of various ICT research domains, such as Robotics and Assisted (Tele-) Heath services, or optimized energy efficient building management while simultaneously automating Renewable Energy Sources use. The Smart Home infrastructure is used as a pilot program for validation / testing of new technologies and services provided by the research community. It is equipped with a multi-sensorial network that measures in real-time almost all parameters that consist open challenges for a modern home / workplace (energy, occupancy, health, etc.). In 2019, the IsZEB Cluster emerged from the funded support program "Clusters for promoting innovation in local entrepreneurship." from the Regional Operation Programme Central Macedonia 2014-2020. The Cluster has special focus on the Construction sector, aiming to provide tools and guidelines for the entire lifecycle of a smart zero or positive energy building. Comprised of 16 members, including the leading Greek companies and authorities in the field of Smart Energy Buildings, it operates on the triple helix model, providing R&amp;D services, training &amp; education opportunities, ecosystem development, and innovation management The evolution of the nZEB Smart Home into the IsZEB Cluster marks a strategic progression in fostering innovation and collaboration. Building upon the success and expertise of the nZEB Smart Home initiative, the IsZEB Cluster seamlessly continues its mission, bringing together a diverse array of stakeholders. This transition represents a significant step forward in advancing the economy of smart buildings, facilitating research and development services, ecosystem development, and innovation management for businesses ranging from startups to SMEs and industrial entities. The IsZEB Cluster, maintaining the esteemed attribute of a testbed infrastructure inherited from the nZEB Smart Home, plays a pivotal role in driving collaborative projects and initiatives, creating a dynamic ecosystem for the development of the construction sector. European Initiatives: • Horizon 2020 and Horizon Europe: The IsZEB Cluster participates in various EU-funded R&amp;D projects, aimed at advancing sustainable and innovative solutions in the field of smart and zero-energy buildings (e.g. D2EPC, Response, Accept, EUH4D, metabuilding, InCube, SmartLivingEPC, SUSTAIN Eurocluster, SmartSquare). Accordingly, the nZEB Smart Home participates in various H2020 covering diverse technological domains, from robotics and artificial intelligence to energy-efficient buildings and smart healthcare solutions (Plug-N-Harvest, encompass, Greensoul, ACTIVAGE, GHOST, ACROSSING, INTEGRIDY, VICINITY, DELTA, 3DMicroGrid, eDREAM, DRIMPAC, DIH^2, AI DIH Network, SIT4Energy, AMANDA, AI4EU, DIHNET, BIMERR, MEISTER, PLANET, SMILE, IRIS, AIREGIO, SmartLivingEPC and much more) By participating in those projects, IsZEB Cluster &amp; nZEB Smart Home DIH not only stay at the forefront of technological advancements but also play a crucial role in shaping the EU research landscape. These collaborative endeavours allow them to leverage their expertise, state-of-the-art infrastructure, and multi-sensorial network to contribute with valuable insights and solutions to the various projects. • European Digital Innovation Hubs (EDIHs): The IsZEB Cluster and the nZEB Smart Home participate in the EDIHs, specifically engaging with the Synerginn EDIH and the SmartHealth EDIH. As part of the EDIHs, they operate as a Service Provider, offering a state-of-the-art rapid prototyping and novel technologies demonstration infrastructure, providing a tangible asset for businesses, start-ups, and research institutions to test and showcase emerging technologies. National Initiatives: • Smart Specialization Strategy (RIS3): Since its beginning, the nZEB Smart Home was linked with the RIS3 strategy. The RIS3 supported specialization sectors are correlated to Information &amp; Communication Technologies, Energy Applications/Technologies and Microelectronics – Advanced Materials. The activities interrelate mainly to the investment of creation and dissemination of new knowledge and to the investment in Research &amp; Innovation in the above topics. • Co-Financed by Greece &amp; EU (Central Macedonia Initiatives): IsZEB Cluster was established due to its participation in the programme "Cooperative formations for the promotion of innovation in local entrepreneurship". Its purpose was to promote innovation in local entrepreneurship, foster the sharing of facilities and equipment, and encourage the exchange of knowledge and expertise, networking, dissemination of information and cooperation between companies and other organizations of the cluster. Co-financing fund: European Regional Development Fund (ERDF)</t>
@@ -5063,10 +4936,8 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="1" t="inlineStr">
-        <is>
-          <t>MDZ KL</t>
-        </is>
+      <c r="A68" s="1" t="n">
+        <v>66</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
@@ -5120,16 +4991,14 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="1" t="inlineStr">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="inlineStr">
         <is>
           <t>Mittelstand-Digital Zentrum Darmstadt</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>Mittelstand-Digital Zentrum Darmstadt</t>
-        </is>
-      </c>
       <c r="C69" t="inlineStr">
         <is>
           <t>The Mittelstand-Digital Zentrum Darmstadt supports small and medium-sized enterprises (SMEs) in their efforts to digizite their business with hands-on-oriented services. All services provided are fully funded by the Federal Ministry for Economic Affairs and Climate Action and create no additionals costs for the recipient. The service includes initial help and orientation for SMEs as well as the support of specific projects. We are also happy to visit companies and partners on site for events and technical consulting. With our online seminars, we offer easily accessible and flexible entry-level formats. We support SMEs that are operating in the manufaturing sector with six key fields of expertise: 1. digital manufaturing 2. product and service development 3. digital work 4. cybersecurity 5. climate-neutral manufacturing 6. artificial intelligence A total of seven partners are pooling their expertise in the Mittelstand-Digital Zentrum Darmstadt: The Institute PTW at TU Darmstadt, the Institutes IAD and PtU and PLCM, the Fraunhofer LBF, the Fraunhofer IGD in Darmstadt and the Chamber of Industry and Commerce in Darmstadt. The Mittelstand-Digital Zentrum Darmstadt is one of 29 centers nationwide in the Mittelstand-Digital network. With Mittelstand-Digital, the Federal Ministry for Economic Affairs and Energy supports digitalization in small and medium-sized enterprises. By working together in the network, we can offer cross-center support and always put SMEs in touch with the right partner if required.</t>
@@ -5177,16 +5046,14 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="1" t="inlineStr">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="inlineStr">
         <is>
           <t>Mittelstand-Digital Zentrum Rostock</t>
         </is>
       </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>Mittelstand-Digital Zentrum Rostock</t>
-        </is>
-      </c>
       <c r="C70" t="inlineStr">
         <is>
           <t>The Mittelstand-Digital Zentrum Rostock offers professional support and tailored solutions to small and medium-sized enterprises in Mecklenburg-Western Pomerania, that enable them to benefit from the digital transformation. With our experts and network we want to help companies to turn existing challenges into opportunities. With free events, practical presentations, certified trainings, and individual digital projects, we support SMEs on their journey into a digital company. The Mittelstand-Digital Zentrum Rostock particularly focuses on companies related to the following sectors: healthcare, medical technology, tourism, health tourism, and construction industry. Keywords: AI knowledge transfer, free workshops, e-learning, digitalchecks, demonstrations, networking, keynotes</t>
@@ -5234,16 +5101,14 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="1" t="inlineStr">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="inlineStr">
         <is>
           <t>Mittelstand-Digital Zentrum WertNetzWerke</t>
         </is>
       </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>Mittelstand-Digital Zentrum WertNetzWerke</t>
-        </is>
-      </c>
       <c r="C71" t="inlineStr">
         <is>
           <t>The Mittelstand-Digital Zentrum WertNetzWerke, funded by the Federal Ministry of Economics, supports SMEs free of charge and in a provider-neutral manner in the development and implementation of sustainable and digital business ideas. The Mittelstand-Digital Zentrum WertNetzWerke, funded by the Federal Ministry of Economics, supports SMEs free of charge and in a provider-neutral manner in the development and implementation of sustainable and digital business ideas.</t>
@@ -5291,10 +5156,8 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="1" t="inlineStr">
-        <is>
-          <t>Robocoast</t>
-        </is>
+      <c r="A72" s="1" t="n">
+        <v>70</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
@@ -5348,10 +5211,8 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="1" t="inlineStr">
-        <is>
-          <t>pro_digital</t>
-        </is>
+      <c r="A73" s="1" t="n">
+        <v>71</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
@@ -5413,10 +5274,8 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="1" t="inlineStr">
-        <is>
-          <t>EDUPARK</t>
-        </is>
+      <c r="A74" s="1" t="n">
+        <v>72</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
@@ -5470,10 +5329,8 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="1" t="inlineStr">
-        <is>
-          <t>InnovationAmp</t>
-        </is>
+      <c r="A75" s="1" t="n">
+        <v>73</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
@@ -5523,10 +5380,8 @@
       <c r="K75" t="inlineStr"/>
     </row>
     <row r="76">
-      <c r="A76" s="1" t="inlineStr">
-        <is>
-          <t>digihub.li</t>
-        </is>
+      <c r="A76" s="1" t="n">
+        <v>74</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
@@ -5596,10 +5451,8 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="1" t="inlineStr">
-        <is>
-          <t>CETMA-DIHSME</t>
-        </is>
+      <c r="A77" s="1" t="n">
+        <v>75</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
@@ -5660,10 +5513,8 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="1" t="inlineStr">
-        <is>
-          <t>CeADAR</t>
-        </is>
+      <c r="A78" s="1" t="n">
+        <v>76</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
@@ -5717,10 +5568,8 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="1" t="inlineStr">
-        <is>
-          <t>INNOFEIT EDIH</t>
-        </is>
+      <c r="A79" s="1" t="n">
+        <v>77</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
@@ -5777,10 +5626,8 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="1" t="inlineStr">
-        <is>
-          <t>EDIH Anadolu</t>
-        </is>
+      <c r="A80" s="1" t="n">
+        <v>78</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
@@ -5837,10 +5684,8 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" s="1" t="inlineStr">
-        <is>
-          <t>DIU</t>
-        </is>
+      <c r="A81" s="1" t="n">
+        <v>79</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
@@ -5894,10 +5739,8 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" s="1" t="inlineStr">
-        <is>
-          <t>DigitalTech EDIH</t>
-        </is>
+      <c r="A82" s="1" t="n">
+        <v>80</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
@@ -5947,10 +5790,8 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" s="1" t="inlineStr">
-        <is>
-          <t>SEEU TechPark</t>
-        </is>
+      <c r="A83" s="1" t="n">
+        <v>81</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
@@ -6004,10 +5845,8 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" s="1" t="inlineStr">
-        <is>
-          <t>FxC</t>
-        </is>
+      <c r="A84" s="1" t="n">
+        <v>82</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
@@ -6065,10 +5904,8 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" s="1" t="inlineStr">
-        <is>
-          <t>OK!Thess</t>
-        </is>
+      <c r="A85" s="1" t="n">
+        <v>83</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
@@ -6122,10 +5959,8 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" s="1" t="inlineStr">
-        <is>
-          <t>MDZH</t>
-        </is>
+      <c r="A86" s="1" t="n">
+        <v>84</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
@@ -6179,10 +6014,8 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" s="1" t="inlineStr">
-        <is>
-          <t>Mittelstand-Digital Zentrum Schleswig-Holstein</t>
-        </is>
+      <c r="A87" s="1" t="n">
+        <v>85</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
@@ -6238,16 +6071,14 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="1" t="inlineStr">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="inlineStr">
         <is>
           <t>Transferstelle Cybersicherheit im Mittelstand</t>
         </is>
       </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>Transferstelle Cybersicherheit im Mittelstand</t>
-        </is>
-      </c>
       <c r="C88" t="inlineStr">
         <is>
           <t>The Cybersecurity Transfer Office for SMEs supports small and medium-sized enterprises, craft businesses and start-ups free of charge in preventing, detecting and responding to cyberattacks. Through information and qualification formats, numerous events throughout Germany, a detection and response platform for cyberattacks and a broad network of partners, we aim to increase the level of cybersecurity in SMEs and thus make German SMEs more resilient. The SME sector, represented by BVMW e. V., acts as consortium leader of the project and works closely with the specialist partners FZI Forschungszentrum Informatik in Karlsruhe, Leibniz Universität Hannover - Institut für Berufspädagogik und Erwachsenenbildung and tti Technologietransfer und Innovationsförderung Magdeburg GmbH. The project is supported by various partners, including Deutschland sicher im Netz e. V. The SME Digital Network offers comprehensive support for digitalization with the SME Digital Centres, the IT Security in Business funding priority and Digital Now. Small and medium-sized enterprises benefit from concrete practical examples and tailor-made, provider-neutral offers for qualification and IT security. The Federal Ministry for Economic Affairs and Climate Protection enables free use and provides financial subsidies. Keywords: Cyber Security</t>
@@ -6295,10 +6126,8 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" s="1" t="inlineStr">
-        <is>
-          <t>IMECH</t>
-        </is>
+      <c r="A89" s="1" t="n">
+        <v>87</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
@@ -6352,10 +6181,8 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" s="1" t="inlineStr">
-        <is>
-          <t>CATCH atMIND</t>
-        </is>
+      <c r="A90" s="1" t="n">
+        <v>88</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
@@ -6408,10 +6235,8 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" s="1" t="inlineStr">
-        <is>
-          <t>CIH</t>
-        </is>
+      <c r="A91" s="1" t="n">
+        <v>89</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
@@ -6465,10 +6290,8 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" s="1" t="inlineStr">
-        <is>
-          <t>IFARLAB</t>
-        </is>
+      <c r="A92" s="1" t="n">
+        <v>90</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
@@ -6528,16 +6351,14 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" s="1" t="inlineStr">
+      <c r="A93" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" t="inlineStr">
         <is>
           <t>Mittelstand-Digital Zentrum Handel</t>
         </is>
       </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>Mittelstand-Digital Zentrum Handel</t>
-        </is>
-      </c>
       <c r="C93" t="inlineStr">
         <is>
           <t>The Mittelstand-Digital Zentrum Handel is the sector-specific contact point for small and medium-sized retail and wholesale companies in Germany. It supports SMEs in making their business models sustainably future-proof with the help of digital applications and technologies. Funded by the Initiative Mittelstand-Digital of the Federal Ministry of Economics and Climate Protection, the centre is made up of the German Retail Association (HDE), ibi research, EHI Retail Institute, IFH Cologne and the German Research Centre for Artificial Intelligence (DFKI).</t>
@@ -6585,10 +6406,8 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" s="1" t="inlineStr">
-        <is>
-          <t>Tuscany X.0</t>
-        </is>
+      <c r="A94" s="1" t="n">
+        <v>92</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
@@ -6638,10 +6457,8 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" s="1" t="inlineStr">
-        <is>
-          <t>DIHBAI-TUR</t>
-        </is>
+      <c r="A95" s="1" t="n">
+        <v>93</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
@@ -6695,10 +6512,8 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" s="1" t="inlineStr">
-        <is>
-          <t>Crowd in Motion</t>
-        </is>
+      <c r="A96" s="1" t="n">
+        <v>94</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
@@ -6752,10 +6567,8 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="1" t="inlineStr">
-        <is>
-          <t>CYBER4All STAR</t>
-        </is>
+      <c r="A97" s="1" t="n">
+        <v>95</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
@@ -6810,10 +6623,8 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" s="1" t="inlineStr">
-        <is>
-          <t>EDIH NN</t>
-        </is>
+      <c r="A98" s="1" t="n">
+        <v>96</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
@@ -6877,10 +6688,8 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" s="1" t="inlineStr">
-        <is>
-          <t>EDIH Saxony</t>
-        </is>
+      <c r="A99" s="1" t="n">
+        <v>97</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
@@ -6930,10 +6739,8 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" s="1" t="inlineStr">
-        <is>
-          <t>EDIH innovATE</t>
-        </is>
+      <c r="A100" s="1" t="n">
+        <v>98</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
@@ -6987,10 +6794,8 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" s="1" t="inlineStr">
-        <is>
-          <t>EDIH-IS</t>
-        </is>
+      <c r="A101" s="1" t="n">
+        <v>99</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
@@ -7040,10 +6845,8 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" s="1" t="inlineStr">
-        <is>
-          <t>FIT EDIH</t>
-        </is>
+      <c r="A102" s="1" t="n">
+        <v>100</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
@@ -7102,16 +6905,14 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="1" t="inlineStr">
+      <c r="A103" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="B103" t="inlineStr">
         <is>
           <t>Mittelstand-Digital Zentrum Bau</t>
         </is>
       </c>
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>Mittelstand-Digital Zentrum Bau</t>
-        </is>
-      </c>
       <c r="C103" t="inlineStr">
         <is>
           <t>With the Mittelstand-Digital Zentrum Bau, small and medium-sized companies in the construction and real estate industry have a strong partner who supports them on their way to the digital and sustainable future. We impart digital skills, promote the implementation of practical solutions and network those involved in the process. Our provider-neutral and free offers cover the entire construction value chain by combining digitalization and sustainability: from project development to dismantling. As a "Mittalestand Digital Zentrum", we are part of the national network of medium-sized digital centers with the aim of supporting small and medium-sized companies in their digital transformation.</t>
@@ -7159,16 +6960,14 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" s="1" t="inlineStr">
+      <c r="A104" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="B104" t="inlineStr">
         <is>
           <t>Mittelstand-Digital Zentrum Magdeburg</t>
         </is>
       </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>Mittelstand-Digital Zentrum Magdeburg</t>
-        </is>
-      </c>
       <c r="C104" t="inlineStr">
         <is>
           <t>The Mittelstand-Digital Zentrum Magdeburg supports small and medium-sized enterprises (SMEs for short) on their digital transformation journey towards competitive products and services, innovative business models and efficient value creation networks. We empower companies and craft businesses and are a cross-industry contact point in the Experimental Factory in Magdeburg.</t>
@@ -7216,10 +7015,8 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" s="1" t="inlineStr">
-        <is>
-          <t>SYNERGiNN EDIH</t>
-        </is>
+      <c r="A105" s="1" t="n">
+        <v>103</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
@@ -7273,16 +7070,14 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" s="1" t="inlineStr">
+      <c r="A106" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="B106" t="inlineStr">
         <is>
           <t>FIWARE Space</t>
         </is>
       </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>FIWARE Space</t>
-        </is>
-      </c>
       <c r="C106" t="inlineStr">
         <is>
           <t>As a DIH associated to the Badajoz Provincial Council (public administration for the Province of Badajoz, Spain) and its digitalization project, Badajoz Es Más, the FIWARE Space center has carried out a wide range of activities aimed at citizens, local administrations and local companies (particularly SMEs and Start-Ups), always focusing on the topics of Digital Transformation and Smart Technologies. As previously mentioned, the FIWARE Space center is part of the Badajoz Provincial Council, and as such all its activities fall within the digitalization efforts carried out by the provincial administration.</t>
@@ -7330,10 +7125,8 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" s="1" t="inlineStr">
-        <is>
-          <t>ADi4SMEs</t>
-        </is>
+      <c r="A107" s="1" t="n">
+        <v>105</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
@@ -7387,10 +7180,8 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" s="1" t="inlineStr">
-        <is>
-          <t>SIH</t>
-        </is>
+      <c r="A108" s="1" t="n">
+        <v>106</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
@@ -7444,10 +7235,8 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" s="1" t="inlineStr">
-        <is>
-          <t>LUBDIGHUB</t>
-        </is>
+      <c r="A109" s="1" t="n">
+        <v>107</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
@@ -7497,10 +7286,8 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" s="1" t="inlineStr">
-        <is>
-          <t>SEDIH</t>
-        </is>
+      <c r="A110" s="1" t="n">
+        <v>108</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
@@ -7554,10 +7341,8 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" s="1" t="inlineStr">
-        <is>
-          <t>NEST</t>
-        </is>
+      <c r="A111" s="1" t="n">
+        <v>109</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
@@ -7607,10 +7392,8 @@
       </c>
     </row>
     <row r="112">
-      <c r="A112" s="1" t="inlineStr">
-        <is>
-          <t>FAIR</t>
-        </is>
+      <c r="A112" s="1" t="n">
+        <v>110</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
@@ -7665,10 +7448,8 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" s="1" t="inlineStr">
-        <is>
-          <t>LIH</t>
-        </is>
+      <c r="A113" s="1" t="n">
+        <v>111</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
@@ -7733,10 +7514,8 @@
       </c>
     </row>
     <row r="114">
-      <c r="A114" s="1" t="inlineStr">
-        <is>
-          <t>Smart Secure Cities</t>
-        </is>
+      <c r="A114" s="1" t="n">
+        <v>112</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
@@ -7786,10 +7565,8 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" s="1" t="inlineStr">
-        <is>
-          <t>WAMA EDIH</t>
-        </is>
+      <c r="A115" s="1" t="n">
+        <v>113</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
@@ -7846,10 +7623,8 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" s="1" t="inlineStr">
-        <is>
-          <t>DIGIS3</t>
-        </is>
+      <c r="A116" s="1" t="n">
+        <v>114</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
@@ -7903,10 +7678,8 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" s="1" t="inlineStr">
-        <is>
-          <t>DIS-HUB</t>
-        </is>
+      <c r="A117" s="1" t="n">
+        <v>115</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
@@ -7960,10 +7733,8 @@
       </c>
     </row>
     <row r="118">
-      <c r="A118" s="1" t="inlineStr">
-        <is>
-          <t>WIN2EDIH</t>
-        </is>
+      <c r="A118" s="1" t="n">
+        <v>116</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
@@ -8020,10 +7791,8 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" s="1" t="inlineStr">
-        <is>
-          <t>AgrInnovate EDIH</t>
-        </is>
+      <c r="A119" s="1" t="n">
+        <v>117</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
@@ -8080,10 +7849,8 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="1" t="inlineStr">
-        <is>
-          <t>CIPS</t>
-        </is>
+      <c r="A120" s="1" t="n">
+        <v>118</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
@@ -8137,10 +7904,8 @@
       </c>
     </row>
     <row r="121">
-      <c r="A121" s="1" t="inlineStr">
-        <is>
-          <t>DIG-4K</t>
-        </is>
+      <c r="A121" s="1" t="n">
+        <v>119</v>
       </c>
       <c r="B121" t="inlineStr">
         <is>
@@ -8196,10 +7961,8 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" s="1" t="inlineStr">
-        <is>
-          <t>MontEDIH</t>
-        </is>
+      <c r="A122" s="1" t="n">
+        <v>120</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
@@ -8250,10 +8013,8 @@
       </c>
     </row>
     <row r="123">
-      <c r="A123" s="1" t="inlineStr">
-        <is>
-          <t>DigiAgriFood</t>
-        </is>
+      <c r="A123" s="1" t="n">
+        <v>121</v>
       </c>
       <c r="B123" t="inlineStr">
         <is>
@@ -8303,10 +8064,8 @@
       </c>
     </row>
     <row r="124">
-      <c r="A124" s="1" t="inlineStr">
-        <is>
-          <t>GC-EDIH</t>
-        </is>
+      <c r="A124" s="1" t="n">
+        <v>122</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
@@ -8361,10 +8120,8 @@
       </c>
     </row>
     <row r="125">
-      <c r="A125" s="1" t="inlineStr">
-        <is>
-          <t>DigitMak</t>
-        </is>
+      <c r="A125" s="1" t="n">
+        <v>123</v>
       </c>
       <c r="B125" t="inlineStr">
         <is>
@@ -8419,10 +8176,8 @@
       </c>
     </row>
     <row r="126">
-      <c r="A126" s="1" t="inlineStr">
-        <is>
-          <t>AI4DigiT</t>
-        </is>
+      <c r="A126" s="1" t="n">
+        <v>124</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
@@ -8473,10 +8228,8 @@
       </c>
     </row>
     <row r="127">
-      <c r="A127" s="1" t="inlineStr">
-        <is>
-          <t>EDIH BRETAGNE</t>
-        </is>
+      <c r="A127" s="1" t="n">
+        <v>125</v>
       </c>
       <c r="B127" t="inlineStr">
         <is>
@@ -8526,10 +8279,8 @@
       </c>
     </row>
     <row r="128">
-      <c r="A128" s="1" t="inlineStr">
-        <is>
-          <t>EDIH Kyiv HiTech</t>
-        </is>
+      <c r="A128" s="1" t="n">
+        <v>126</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
@@ -8584,10 +8335,8 @@
       </c>
     </row>
     <row r="129">
-      <c r="A129" s="1" t="inlineStr">
-        <is>
-          <t>ENTIRE</t>
-        </is>
+      <c r="A129" s="1" t="n">
+        <v>127</v>
       </c>
       <c r="B129" t="inlineStr">
         <is>
@@ -8641,10 +8390,8 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" s="1" t="inlineStr">
-        <is>
-          <t>4PDIH</t>
-        </is>
+      <c r="A130" s="1" t="n">
+        <v>128</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
@@ -8698,10 +8445,8 @@
       </c>
     </row>
     <row r="131">
-      <c r="A131" s="1" t="inlineStr">
-        <is>
-          <t>IRIS</t>
-        </is>
+      <c r="A131" s="1" t="n">
+        <v>129</v>
       </c>
       <c r="B131" t="inlineStr">
         <is>
@@ -8755,10 +8500,8 @@
       </c>
     </row>
     <row r="132">
-      <c r="A132" s="1" t="inlineStr">
-        <is>
-          <t>InnDIH</t>
-        </is>
+      <c r="A132" s="1" t="n">
+        <v>130</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
@@ -8814,10 +8557,8 @@
       </c>
     </row>
     <row r="133">
-      <c r="A133" s="1" t="inlineStr">
-        <is>
-          <t>AGORA DIH</t>
-        </is>
+      <c r="A133" s="1" t="n">
+        <v>131</v>
       </c>
       <c r="B133" t="inlineStr">
         <is>
@@ -8871,10 +8612,8 @@
       </c>
     </row>
     <row r="134">
-      <c r="A134" s="1" t="inlineStr">
-        <is>
-          <t>STP Belgrade</t>
-        </is>
+      <c r="A134" s="1" t="n">
+        <v>132</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
@@ -8928,10 +8667,8 @@
       </c>
     </row>
     <row r="135">
-      <c r="A135" s="1" t="inlineStr">
-        <is>
-          <t>BITF</t>
-        </is>
+      <c r="A135" s="1" t="n">
+        <v>133</v>
       </c>
       <c r="B135" t="inlineStr">
         <is>
@@ -8986,10 +8723,8 @@
       </c>
     </row>
     <row r="136">
-      <c r="A136" s="1" t="inlineStr">
-        <is>
-          <t>DIH ONEX</t>
-        </is>
+      <c r="A136" s="1" t="n">
+        <v>134</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
@@ -9044,10 +8779,8 @@
       </c>
     </row>
     <row r="137">
-      <c r="A137" s="1" t="inlineStr">
-        <is>
-          <t>SCDI proposal</t>
-        </is>
+      <c r="A137" s="1" t="n">
+        <v>135</v>
       </c>
       <c r="B137" t="inlineStr">
         <is>
@@ -9101,10 +8834,8 @@
       </c>
     </row>
     <row r="138">
-      <c r="A138" s="1" t="inlineStr">
-        <is>
-          <t>Tech4EfficiencyEDIH</t>
-        </is>
+      <c r="A138" s="1" t="n">
+        <v>136</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
@@ -9158,10 +8889,8 @@
       </c>
     </row>
     <row r="139">
-      <c r="A139" s="1" t="inlineStr">
-        <is>
-          <t>CIDAI</t>
-        </is>
+      <c r="A139" s="1" t="n">
+        <v>137</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
@@ -9215,10 +8944,8 @@
       </c>
     </row>
     <row r="140">
-      <c r="A140" s="1" t="inlineStr">
-        <is>
-          <t>Bayern Innovativ</t>
-        </is>
+      <c r="A140" s="1" t="n">
+        <v>138</v>
       </c>
       <c r="B140" t="inlineStr">
         <is>
@@ -9272,16 +8999,14 @@
       </c>
     </row>
     <row r="141">
-      <c r="A141" s="1" t="inlineStr">
+      <c r="A141" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="B141" t="inlineStr">
         <is>
           <t>DIGI2Health</t>
         </is>
       </c>
-      <c r="B141" t="inlineStr">
-        <is>
-          <t>DIGI2Health</t>
-        </is>
-      </c>
       <c r="C141" t="inlineStr">
         <is>
           <t>DIGI2Health is a collaborative project established to address the need for systemic changes in healthcare both within and outside the Czech Republic. It also aims to provide technical and knowledge support for innovations in healthcare. Its core founding members are Palacký University Olomouc, Faculty Hospital Olomouc and Olomouc Region Innovation Center. Recently, the project was relocated to a separate facility because we firmly believe that a crucial aspect of innovation is in-person interaction and ideation. This new facility, Envelopa Hub, now serves as the home not only for project partners but also for innovative companies and student organizations. It provides a dedicated co-working space and experimental laboratories that align with the mission and vision of the project. The project follows the structure of digital innovation hubs defined by the European Commission and is listed in the DIH catalogue. In addition to the main partners of the Digi2Health innovation hub described in detail above, it is worth noting that the hub heavily relies on its other members and collaborating partners. These entities provide us with insights and access, including but not limited to private healthcare, such as Agel - a leading private healthcare provider in Central Europe (https://eu.agel.cz/index.html), and specialized organizations like the Alliance for Telemedicine (https://www.atdz.cz/poslani-a-cile), which brings together key stakeholders in the fields of telemedicine and the digitalization of health and social services. Laboratory of DIGI2Health can offer to SMEs experimental laboratory for devices used in healthcare. For example simulating patient movement in surgeries through technology Wi-Fi kit for indoor UWB signal monitoring, climate chamber for testing electronic devices or electroimpedancy tomograph with 16 chanells. More information you can find on website: www.digi2health.com.</t>
@@ -9329,16 +9054,14 @@
       </c>
     </row>
     <row r="142">
-      <c r="A142" s="1" t="inlineStr">
+      <c r="A142" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="B142" t="inlineStr">
         <is>
           <t>GreenPulse 5.0</t>
         </is>
       </c>
-      <c r="B142" t="inlineStr">
-        <is>
-          <t>GreenPulse 5.0</t>
-        </is>
-      </c>
       <c r="C142" t="inlineStr">
         <is>
           <t>GreenPulse 5.0, coordinated by Pomurje technology park (Slovenia), is dedicated to helping SMEs in manufacturing sector embrace digital innovation for a greener tomorrow. GreenPulse 5.0 serves as a catalyst for SMEs seeking cutting-edge technologies to enhance their manufacturing processes. Whether you're in electronic manufacturing, food &amp; beverage processing, pharmaceuticals, metal processing, plastics, machinery &amp; equipment, or building materials &amp; furniture, GreenPulse 5.0 is your gateway to unlocking the potential of your SME with sustainable and state-of-the-art digital technologies. We focus on key areas that drive efficiency, reduce costs, and elevate sustainability. Our hub understands the unique needs of SMEs, offering tailored solutions that fit the scale and requirements of small and medium-sized enterprises. GreenPulse 5.0 is not just a hub; it's your partner in navigating the future of manufacturing. Operating in Eastern Slovenia, GreenPulse 5.0 extends its reach through partnerships with over 200 (E)DIHs across Europe. Join a network that fosters collaboration and innovation beyond borders. Our organizational competencies and resources emanate from proficiency in five distinct technology domains: 1. Digitalization and Connectivity:Internet of Things, Edge Computing, Digital Twin Technology. 2. Automation and Robotics: Robotics and Automation, Collaborative Robots, Artificial Intelligence in Robotics. 3. Data Analytics and Artificial Intelligence: Big Data Analytics, Machine Learning, Predictive Maintenance, 4. Additive Manufacturing, and 3D Printing: 3D Printing/Additive Manufacturing; Rapid Prototyping; Digital Fabrication. 5. Cybersecurity and Digital Trust: Cybersecurity, Blockchain Technology, Security of IoT Devices. From renewable energy adoption to waste reduction technologies, GreenPulse 5.0 supports SMEs in implementing sustainable manufacturing processes. These green technologies play a crucial role in addressing environmental challenges, promoting sustainability, and helping the manufacturing industry reduce its ecological footprint. Combining these technologies with digital solutions can create a comprehensive approach to green and sustainable manufacturing. Clients can discover green innovations that not only boost efficiency but also align with eco-friendly practices: 1. Renewable Energy Sources: Solar Power, Wind Power, Hydropower. 2. Energy-Efficient Equipment and Processes: Energy-Efficient Motors and Drives, LED Lighting, Heat Recovery Systems. 3. Waste Reduction and Recycling Technologies: Waste-to-Energy Conversion, Closed-Loop Manufacturing Systems, Recycling Technologies. 4. Green Materials and Sustainable Design: Biodegradable Materials, Recycled Materials, Sustainable Packaging 5. Water Conservation Technologies: Water Recycling and Reuse Systems, Water-Efficient Manufacturing Processes, Rainwater Harvesting 6. Carbon Capture and Storage (CCS): Carbon Capture Technologies, Carbon Sequestration 7. Lean Manufacturing Practices: Just-in-Time Manufacturing, Total Quality Management (TQM), Continuous Improvement 8. Green Certification and Standards: ISO 14001 (Environmental Management System); ENERGY STAR Certification Leadership in Energy and Environmental Design (LEED) Why work with GreenPulse 5.0? • Access to the latest digital and green technologies tailored for SMEs. • Collaborative partnerships with leading ICT service providers • Regional focus on Pomurje and Eastern Slovenia. • Extensive network of over 200 partner DIHs across Europe. • Solutions designed to elevate efficiency, reduce costs, and enhance sustainability for SMEs. Join GreenPulse 5.0 on a journey towards a greener, technologically advanced future for your SME. Let's innovate, collaborate, and shape the future of manufacturing together. Pomurje technology Park with its DIH is a full partner in EDIH 4PDIH consortium, offering its services to SMEs, public administration and policy level. We are constantly collaborating with governmental bodies, either through joint organization of events, joint tender preparation,etc. We are also a member of Working group for the establishment of a national Research and development hub, coordinated by SPIRIT Slovenia.</t>
@@ -9386,10 +9109,8 @@
       </c>
     </row>
     <row r="143">
-      <c r="A143" s="1" t="inlineStr">
-        <is>
-          <t>DIH PANNONIA</t>
-        </is>
+      <c r="A143" s="1" t="n">
+        <v>141</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
@@ -9443,10 +9164,8 @@
       </c>
     </row>
     <row r="144">
-      <c r="A144" s="1" t="inlineStr">
-        <is>
-          <t>EDI</t>
-        </is>
+      <c r="A144" s="1" t="n">
+        <v>142</v>
       </c>
       <c r="B144" t="inlineStr">
         <is>
@@ -9500,10 +9219,8 @@
       </c>
     </row>
     <row r="145">
-      <c r="A145" s="1" t="inlineStr">
-        <is>
-          <t>EOSC DIH</t>
-        </is>
+      <c r="A145" s="1" t="n">
+        <v>143</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
@@ -9557,10 +9274,8 @@
       </c>
     </row>
     <row r="146">
-      <c r="A146" s="1" t="inlineStr">
-        <is>
-          <t>ZSA</t>
-        </is>
+      <c r="A146" s="1" t="n">
+        <v>144</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
@@ -9614,10 +9329,8 @@
       </c>
     </row>
     <row r="147">
-      <c r="A147" s="1" t="inlineStr">
-        <is>
-          <t>Innova iHub</t>
-        </is>
+      <c r="A147" s="1" t="n">
+        <v>145</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
@@ -9671,10 +9384,8 @@
       </c>
     </row>
     <row r="148">
-      <c r="A148" s="1" t="inlineStr">
-        <is>
-          <t>Green eDIH</t>
-        </is>
+      <c r="A148" s="1" t="n">
+        <v>146</v>
       </c>
       <c r="B148" t="inlineStr">
         <is>
@@ -9728,10 +9439,8 @@
       </c>
     </row>
     <row r="149">
-      <c r="A149" s="1" t="inlineStr">
-        <is>
-          <t>Innoskart</t>
-        </is>
+      <c r="A149" s="1" t="n">
+        <v>147</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
@@ -9785,10 +9494,8 @@
       </c>
     </row>
     <row r="150">
-      <c r="A150" s="1" t="inlineStr">
-        <is>
-          <t>Novel-T</t>
-        </is>
+      <c r="A150" s="1" t="n">
+        <v>148</v>
       </c>
       <c r="B150" t="inlineStr">
         <is>
@@ -9842,10 +9549,8 @@
       </c>
     </row>
     <row r="151">
-      <c r="A151" s="1" t="inlineStr">
-        <is>
-          <t>Plan4all</t>
-        </is>
+      <c r="A151" s="1" t="n">
+        <v>149</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>
@@ -9899,10 +9604,8 @@
       </c>
     </row>
     <row r="152">
-      <c r="A152" s="1" t="inlineStr">
-        <is>
-          <t>AIR4S</t>
-        </is>
+      <c r="A152" s="1" t="n">
+        <v>150</v>
       </c>
       <c r="B152" t="inlineStr">
         <is>
@@ -9956,10 +9659,8 @@
       </c>
     </row>
     <row r="153">
-      <c r="A153" s="1" t="inlineStr">
-        <is>
-          <t>SMILE-DIH</t>
-        </is>
+      <c r="A153" s="1" t="n">
+        <v>151</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>
@@ -10013,10 +9714,8 @@
       </c>
     </row>
     <row r="154">
-      <c r="A154" s="1" t="inlineStr">
-        <is>
-          <t>Speedhub</t>
-        </is>
+      <c r="A154" s="1" t="n">
+        <v>152</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
@@ -10070,10 +9769,8 @@
       </c>
     </row>
     <row r="155">
-      <c r="A155" s="1" t="inlineStr">
-        <is>
-          <t>SV DIH</t>
-        </is>
+      <c r="A155" s="1" t="n">
+        <v>153</v>
       </c>
       <c r="B155" t="inlineStr">
         <is>
@@ -10127,10 +9824,8 @@
       </c>
     </row>
     <row r="156">
-      <c r="A156" s="1" t="inlineStr">
-        <is>
-          <t>PCUV</t>
-        </is>
+      <c r="A156" s="1" t="n">
+        <v>154</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
@@ -10184,10 +9879,8 @@
       </c>
     </row>
     <row r="157">
-      <c r="A157" s="1" t="inlineStr">
-        <is>
-          <t>Next-Gen-BIoTechEDIH</t>
-        </is>
+      <c r="A157" s="1" t="n">
+        <v>155</v>
       </c>
       <c r="B157" t="inlineStr">
         <is>
@@ -10237,10 +9930,8 @@
       </c>
     </row>
     <row r="158">
-      <c r="A158" s="1" t="inlineStr">
-        <is>
-          <t>AzoresDIH</t>
-        </is>
+      <c r="A158" s="1" t="n">
+        <v>156</v>
       </c>
       <c r="B158" t="inlineStr">
         <is>
@@ -10294,10 +9985,8 @@
       </c>
     </row>
     <row r="159">
-      <c r="A159" s="1" t="inlineStr">
-        <is>
-          <t>AgroDigiRise</t>
-        </is>
+      <c r="A159" s="1" t="n">
+        <v>157</v>
       </c>
       <c r="B159" t="inlineStr">
         <is>
@@ -10351,10 +10040,8 @@
       </c>
     </row>
     <row r="160">
-      <c r="A160" s="1" t="inlineStr">
-        <is>
-          <t>AgrotechDIH</t>
-        </is>
+      <c r="A160" s="1" t="n">
+        <v>158</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
@@ -10408,10 +10095,8 @@
       </c>
     </row>
     <row r="161">
-      <c r="A161" s="1" t="inlineStr">
-        <is>
-          <t>AsDIH</t>
-        </is>
+      <c r="A161" s="1" t="n">
+        <v>159</v>
       </c>
       <c r="B161" t="inlineStr">
         <is>
@@ -10465,10 +10150,8 @@
       </c>
     </row>
     <row r="162">
-      <c r="A162" s="1" t="inlineStr">
-        <is>
-          <t>CD-EDIH</t>
-        </is>
+      <c r="A162" s="1" t="n">
+        <v>160</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>
@@ -10529,10 +10212,8 @@
       </c>
     </row>
     <row r="163">
-      <c r="A163" s="1" t="inlineStr">
-        <is>
-          <t>CHEDIH</t>
-        </is>
+      <c r="A163" s="1" t="n">
+        <v>161</v>
       </c>
       <c r="B163" t="inlineStr">
         <is>
@@ -10586,10 +10267,8 @@
       </c>
     </row>
     <row r="164">
-      <c r="A164" s="1" t="inlineStr">
-        <is>
-          <t>CITAH</t>
-        </is>
+      <c r="A164" s="1" t="n">
+        <v>162</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
@@ -10643,10 +10322,8 @@
       </c>
     </row>
     <row r="165">
-      <c r="A165" s="1" t="inlineStr">
-        <is>
-          <t>CROBOHUBplusplus</t>
-        </is>
+      <c r="A165" s="1" t="n">
+        <v>163</v>
       </c>
       <c r="B165" t="inlineStr">
         <is>
@@ -10696,10 +10373,8 @@
       </c>
     </row>
     <row r="166">
-      <c r="A166" s="1" t="inlineStr">
-        <is>
-          <t>Cantabria DIH</t>
-        </is>
+      <c r="A166" s="1" t="n">
+        <v>164</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
@@ -10749,10 +10424,8 @@
       </c>
     </row>
     <row r="167">
-      <c r="A167" s="1" t="inlineStr">
-        <is>
-          <t>DATAlife</t>
-        </is>
+      <c r="A167" s="1" t="n">
+        <v>165</v>
       </c>
       <c r="B167" t="inlineStr">
         <is>
@@ -10802,10 +10475,8 @@
       </c>
     </row>
     <row r="168">
-      <c r="A168" s="1" t="inlineStr">
-        <is>
-          <t>DIH-bio</t>
-        </is>
+      <c r="A168" s="1" t="n">
+        <v>166</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
@@ -10859,10 +10530,8 @@
       </c>
     </row>
     <row r="169">
-      <c r="A169" s="1" t="inlineStr">
-        <is>
-          <t>DiVA</t>
-        </is>
+      <c r="A169" s="1" t="n">
+        <v>167</v>
       </c>
       <c r="B169" t="inlineStr">
         <is>
@@ -10916,10 +10585,8 @@
       </c>
     </row>
     <row r="170">
-      <c r="A170" s="1" t="inlineStr">
-        <is>
-          <t>DiGiNN</t>
-        </is>
+      <c r="A170" s="1" t="n">
+        <v>168</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>
@@ -10973,10 +10640,8 @@
       </c>
     </row>
     <row r="171">
-      <c r="A171" s="1" t="inlineStr">
-        <is>
-          <t>HSL</t>
-        </is>
+      <c r="A171" s="1" t="n">
+        <v>169</v>
       </c>
       <c r="B171" t="inlineStr">
         <is>
@@ -11030,10 +10695,8 @@
       </c>
     </row>
     <row r="172">
-      <c r="A172" s="1" t="inlineStr">
-        <is>
-          <t>MDZT</t>
-        </is>
+      <c r="A172" s="1" t="n">
+        <v>170</v>
       </c>
       <c r="B172" t="inlineStr">
         <is>
@@ -11087,10 +10750,8 @@
       </c>
     </row>
     <row r="173">
-      <c r="A173" s="1" t="inlineStr">
-        <is>
-          <t>SmartAttica-AtHeNAI</t>
-        </is>
+      <c r="A173" s="1" t="n">
+        <v>171</v>
       </c>
       <c r="B173" t="inlineStr">
         <is>
@@ -11142,10 +10803,8 @@
       </c>
     </row>
     <row r="174">
-      <c r="A174" s="1" t="inlineStr">
-        <is>
-          <t>EDI Confcommercio</t>
-        </is>
+      <c r="A174" s="1" t="n">
+        <v>172</v>
       </c>
       <c r="B174" t="inlineStr">
         <is>
@@ -11199,10 +10858,8 @@
       </c>
     </row>
     <row r="175">
-      <c r="A175" s="1" t="inlineStr">
-        <is>
-          <t>NEURAL</t>
-        </is>
+      <c r="A175" s="1" t="n">
+        <v>173</v>
       </c>
       <c r="B175" t="inlineStr">
         <is>
@@ -11252,10 +10909,8 @@
       </c>
     </row>
     <row r="176">
-      <c r="A176" s="1" t="inlineStr">
-        <is>
-          <t>CIDIHUB</t>
-        </is>
+      <c r="A176" s="1" t="n">
+        <v>174</v>
       </c>
       <c r="B176" t="inlineStr">
         <is>
@@ -11309,16 +10964,14 @@
       </c>
     </row>
     <row r="177">
-      <c r="A177" s="1" t="inlineStr">
+      <c r="A177" s="1" t="n">
+        <v>175</v>
+      </c>
+      <c r="B177" t="inlineStr">
         <is>
           <t>Mittelstand-Digital Zentrum Augsburg</t>
         </is>
       </c>
-      <c r="B177" t="inlineStr">
-        <is>
-          <t>Mittelstand-Digital Zentrum Augsburg</t>
-        </is>
-      </c>
       <c r="C177" t="inlineStr">
         <is>
           <t>-- Wir unterstützen kleine und mittlere Unternehmen sowie das Handwerk mit kostenfreien Angeboten auf ihrem Weg in die Digitalisierung.</t>
@@ -11366,10 +11019,8 @@
       </c>
     </row>
     <row r="178">
-      <c r="A178" s="1" t="inlineStr">
-        <is>
-          <t>SKAI-eDIH</t>
-        </is>
+      <c r="A178" s="1" t="n">
+        <v>176</v>
       </c>
       <c r="B178" t="inlineStr">
         <is>
@@ -11428,10 +11079,8 @@
       </c>
     </row>
     <row r="179">
-      <c r="A179" s="1" t="inlineStr">
-        <is>
-          <t>TKDIH</t>
-        </is>
+      <c r="A179" s="1" t="n">
+        <v>177</v>
       </c>
       <c r="B179" t="inlineStr">
         <is>
@@ -11485,10 +11134,8 @@
       </c>
     </row>
     <row r="180">
-      <c r="A180" s="1" t="inlineStr">
-        <is>
-          <t>AddSmart</t>
-        </is>
+      <c r="A180" s="1" t="n">
+        <v>178</v>
       </c>
       <c r="B180" t="inlineStr">
         <is>
@@ -11541,10 +11188,8 @@
       </c>
     </row>
     <row r="181">
-      <c r="A181" s="1" t="inlineStr">
-        <is>
-          <t>AI EDIH Türkiye</t>
-        </is>
+      <c r="A181" s="1" t="n">
+        <v>179</v>
       </c>
       <c r="B181" t="inlineStr">
         <is>
@@ -11605,10 +11250,8 @@
       </c>
     </row>
     <row r="182">
-      <c r="A182" s="1" t="inlineStr">
-        <is>
-          <t>CentralUkrainianEDIH</t>
-        </is>
+      <c r="A182" s="1" t="n">
+        <v>180</v>
       </c>
       <c r="B182" t="inlineStr">
         <is>
@@ -11662,10 +11305,8 @@
       </c>
     </row>
     <row r="183">
-      <c r="A183" s="1" t="inlineStr">
-        <is>
-          <t>Digital Impulse Hub</t>
-        </is>
+      <c r="A183" s="1" t="n">
+        <v>181</v>
       </c>
       <c r="B183" t="inlineStr">
         <is>
@@ -11719,10 +11360,8 @@
       </c>
     </row>
     <row r="184">
-      <c r="A184" s="1" t="inlineStr">
-        <is>
-          <t>Tech-Stop EDIH</t>
-        </is>
+      <c r="A184" s="1" t="n">
+        <v>182</v>
       </c>
       <c r="B184" t="inlineStr">
         <is>
@@ -11785,10 +11424,8 @@
       </c>
     </row>
     <row r="185">
-      <c r="A185" s="1" t="inlineStr">
-        <is>
-          <t>EDIH OVA</t>
-        </is>
+      <c r="A185" s="1" t="n">
+        <v>183</v>
       </c>
       <c r="B185" t="inlineStr">
         <is>
@@ -11838,10 +11475,8 @@
       </c>
     </row>
     <row r="186">
-      <c r="A186" s="1" t="inlineStr">
-        <is>
-          <t>EDIH Rheinland</t>
-        </is>
+      <c r="A186" s="1" t="n">
+        <v>184</v>
       </c>
       <c r="B186" t="inlineStr">
         <is>
@@ -11891,10 +11526,8 @@
       </c>
     </row>
     <row r="187">
-      <c r="A187" s="1" t="inlineStr">
-        <is>
-          <t>EDIH Suedwest</t>
-        </is>
+      <c r="A187" s="1" t="n">
+        <v>185</v>
       </c>
       <c r="B187" t="inlineStr">
         <is>
@@ -11948,10 +11581,8 @@
       </c>
     </row>
     <row r="188">
-      <c r="A188" s="1" t="inlineStr">
-        <is>
-          <t>EDIH-SILESIA</t>
-        </is>
+      <c r="A188" s="1" t="n">
+        <v>186</v>
       </c>
       <c r="B188" t="inlineStr">
         <is>
@@ -12005,10 +11636,8 @@
       </c>
     </row>
     <row r="189">
-      <c r="A189" s="1" t="inlineStr">
-        <is>
-          <t>EDIH-SNL</t>
-        </is>
+      <c r="A189" s="1" t="n">
+        <v>187</v>
       </c>
       <c r="B189" t="inlineStr">
         <is>
@@ -12062,10 +11691,8 @@
       </c>
     </row>
     <row r="190">
-      <c r="A190" s="1" t="inlineStr">
-        <is>
-          <t>EXPAND</t>
-        </is>
+      <c r="A190" s="1" t="n">
+        <v>188</v>
       </c>
       <c r="B190" t="inlineStr">
         <is>
@@ -12119,10 +11746,8 @@
       </c>
     </row>
     <row r="191">
-      <c r="A191" s="1" t="inlineStr">
-        <is>
-          <t>EXPANDI 4.0</t>
-        </is>
+      <c r="A191" s="1" t="n">
+        <v>189</v>
       </c>
       <c r="B191" t="inlineStr">
         <is>
@@ -12176,10 +11801,8 @@
       </c>
     </row>
     <row r="192">
-      <c r="A192" s="1" t="inlineStr">
-        <is>
-          <t>GreenPowerIT</t>
-        </is>
+      <c r="A192" s="1" t="n">
+        <v>190</v>
       </c>
       <c r="B192" t="inlineStr">
         <is>
@@ -12229,10 +11852,8 @@
       </c>
     </row>
     <row r="193">
-      <c r="A193" s="1" t="inlineStr">
-        <is>
-          <t>MD_Zukunftskultur</t>
-        </is>
+      <c r="A193" s="1" t="n">
+        <v>191</v>
       </c>
       <c r="B193" t="inlineStr">
         <is>
@@ -12286,10 +11907,8 @@
       </c>
     </row>
     <row r="194">
-      <c r="A194" s="1" t="inlineStr">
-        <is>
-          <t>MDZ Fokus Mensch</t>
-        </is>
+      <c r="A194" s="1" t="n">
+        <v>192</v>
       </c>
       <c r="B194" t="inlineStr">
         <is>
@@ -12343,10 +11962,8 @@
       </c>
     </row>
     <row r="195">
-      <c r="A195" s="1" t="inlineStr">
-        <is>
-          <t>MDZ Smarte Kreislaeufe</t>
-        </is>
+      <c r="A195" s="1" t="n">
+        <v>193</v>
       </c>
       <c r="B195" t="inlineStr">
         <is>
@@ -12400,10 +12017,8 @@
       </c>
     </row>
     <row r="196">
-      <c r="A196" s="1" t="inlineStr">
-        <is>
-          <t>MDZ Spreeland</t>
-        </is>
+      <c r="A196" s="1" t="n">
+        <v>194</v>
       </c>
       <c r="B196" t="inlineStr">
         <is>
@@ -12457,10 +12072,8 @@
       </c>
     </row>
     <row r="197">
-      <c r="A197" s="1" t="inlineStr">
-        <is>
-          <t>MDZLR</t>
-        </is>
+      <c r="A197" s="1" t="n">
+        <v>195</v>
       </c>
       <c r="B197" t="inlineStr">
         <is>
@@ -12514,16 +12127,14 @@
       </c>
     </row>
     <row r="198">
-      <c r="A198" s="1" t="inlineStr">
+      <c r="A198" s="1" t="n">
+        <v>196</v>
+      </c>
+      <c r="B198" t="inlineStr">
         <is>
           <t>Mittelstand-Digital Zentrum Chemnitz</t>
         </is>
       </c>
-      <c r="B198" t="inlineStr">
-        <is>
-          <t>Mittelstand-Digital Zentrum Chemnitz</t>
-        </is>
-      </c>
       <c r="C198" t="inlineStr">
         <is>
           <t>The Mittelstand-Digital Center Chemnitz is a contact point for small and medium-sized companies from all over Saxony that are interested in the topics of digitalization and artificial intelligence. The aim is to introduce companies to forward-looking topics, strengthen their digital expertise and support the development of new strategies. The center therefore focuses on digital business models and technological solutions, including the application of artificial intelligence. The focus is also on topics such as IT security, law and sustainability. The Mittelstand-Digital Center Chemnitz offers a wide range of free and provider-neutral services. These include workshops, seminars, guidelines and project support. All offers are aimed at both beginners and experienced entrepreneurs. Demonstrators are used in test and training environments to try out individual digitalization solutions. These illustrate how digital solutions can be implemented in practice. The center works closely with a network of partners. This cooperation enables comprehensive support for companies in the field of digitalization and artificial intelligence.</t>
@@ -12571,16 +12182,14 @@
       </c>
     </row>
     <row r="199">
-      <c r="A199" s="1" t="inlineStr">
+      <c r="A199" s="1" t="n">
+        <v>197</v>
+      </c>
+      <c r="B199" t="inlineStr">
         <is>
           <t>Mittelstand-Digital Zentrum Rheinland</t>
         </is>
       </c>
-      <c r="B199" t="inlineStr">
-        <is>
-          <t>Mittelstand-Digital Zentrum Rheinland</t>
-        </is>
-      </c>
       <c r="C199" t="inlineStr">
         <is>
           <t>The Mittelstand-Digital Zentrum Rheinland supports SMEs in the Rhineland to make their companies ready for the future by themselves, using digitalization methods and technologies. The Mittelstand-Digital Zentrum Rheinland also provides help in the field of AI especially in the production, construction and trade sectors. The Mittelstand-Digital Zentrum Rheinland is part of the Mittelstand-Digital initiative.</t>
@@ -12628,16 +12237,14 @@
       </c>
     </row>
     <row r="200">
-      <c r="A200" s="1" t="inlineStr">
+      <c r="A200" s="1" t="n">
+        <v>198</v>
+      </c>
+      <c r="B200" t="inlineStr">
         <is>
           <t>Mittelstand-Digital Zentrum Saarbrücken</t>
         </is>
       </c>
-      <c r="B200" t="inlineStr">
-        <is>
-          <t>Mittelstand-Digital Zentrum Saarbrücken</t>
-        </is>
-      </c>
       <c r="C200" t="inlineStr">
         <is>
           <t>The Mittelstand-Digital Zentrum Saarbrücken supports small and medium-sized enterprises (SMEs) in the digital transformation. The center is part of the initiative “Mittelstand-Digital“ by the German Federal Ministry for Economic Affairs and Climate Action (www.mittelstand-digital.de).</t>
@@ -12685,10 +12292,8 @@
       </c>
     </row>
     <row r="201">
-      <c r="A201" s="1" t="inlineStr">
-        <is>
-          <t>DUTIREG</t>
-        </is>
+      <c r="A201" s="1" t="n">
+        <v>199</v>
       </c>
       <c r="B201" t="inlineStr">
         <is>
@@ -12742,10 +12347,8 @@
       </c>
     </row>
     <row r="202">
-      <c r="A202" s="1" t="inlineStr">
-        <is>
-          <t>PBN</t>
-        </is>
+      <c r="A202" s="1" t="n">
+        <v>200</v>
       </c>
       <c r="B202" t="inlineStr">
         <is>
@@ -12799,10 +12402,8 @@
       </c>
     </row>
     <row r="203">
-      <c r="A203" s="1" t="inlineStr">
-        <is>
-          <t>BRH</t>
-        </is>
+      <c r="A203" s="1" t="n">
+        <v>201</v>
       </c>
       <c r="B203" t="inlineStr">
         <is>
@@ -12857,10 +12458,8 @@
       </c>
     </row>
     <row r="204">
-      <c r="A204" s="1" t="inlineStr">
-        <is>
-          <t>INNOFEIT</t>
-        </is>
+      <c r="A204" s="1" t="n">
+        <v>202</v>
       </c>
       <c r="B204" t="inlineStr">
         <is>
@@ -12916,10 +12515,8 @@
       </c>
     </row>
     <row r="205">
-      <c r="A205" s="1" t="inlineStr">
-        <is>
-          <t>WRO4digITal</t>
-        </is>
+      <c r="A205" s="1" t="n">
+        <v>203</v>
       </c>
       <c r="B205" t="inlineStr">
         <is>
@@ -12973,10 +12570,8 @@
       </c>
     </row>
     <row r="206">
-      <c r="A206" s="1" t="inlineStr">
-        <is>
-          <t>h4i</t>
-        </is>
+      <c r="A206" s="1" t="n">
+        <v>204</v>
       </c>
       <c r="B206" t="inlineStr">
         <is>
@@ -13030,10 +12625,8 @@
       </c>
     </row>
     <row r="207">
-      <c r="A207" s="1" t="inlineStr">
-        <is>
-          <t>Advanced Manufacturing Digital Innovation Hub</t>
-        </is>
+      <c r="A207" s="1" t="n">
+        <v>205</v>
       </c>
       <c r="B207" t="inlineStr">
         <is>
@@ -13087,10 +12680,8 @@
       </c>
     </row>
     <row r="208">
-      <c r="A208" s="1" t="inlineStr">
-        <is>
-          <t>AIVHY Industry 4.0 Innovation Hub</t>
-        </is>
+      <c r="A208" s="1" t="n">
+        <v>206</v>
       </c>
       <c r="B208" t="inlineStr">
         <is>
@@ -13144,10 +12735,8 @@
       </c>
     </row>
     <row r="209">
-      <c r="A209" s="1" t="inlineStr">
-        <is>
-          <t>CMH</t>
-        </is>
+      <c r="A209" s="1" t="n">
+        <v>207</v>
       </c>
       <c r="B209" t="inlineStr">
         <is>
@@ -13201,16 +12790,14 @@
       </c>
     </row>
     <row r="210">
-      <c r="A210" s="1" t="inlineStr">
+      <c r="A210" s="1" t="n">
+        <v>208</v>
+      </c>
+      <c r="B210" t="inlineStr">
         <is>
           <t>DIH Veneto</t>
         </is>
       </c>
-      <c r="B210" t="inlineStr">
-        <is>
-          <t>DIH Veneto</t>
-        </is>
-      </c>
       <c r="C210" t="inlineStr">
         <is>
           <t>The DIH Veneto is managed by Confindustria Veneto SIAV Srl, the service company of Confindustria Veneto. It operates at a regional level in close connection with the "territorial antennas" set up by the Industrial Associations of the Veneto provinces and the provincial DIHs of Confindustria. The objective of DIH Veneto is to support the business system in the digital transition process through a structured series of initiatives, activities and services: • Awareness-raising and training on the opportunities related to the application of 4.0 technologies through the organisation of seminars, workshops, training courses and study visits; • Management animation and promotion of the regional network of Industry 4.0 showcase factories https://100luoghi.industria40veneto.it/ • Research and studies in the field of 4.0 aimed at promoting and developing the managerial culture • Digital maturity assessment: support in the use of digital maturity assessment tools, the definition of the roadmap for the digital transformation of business processes and accompaniment in the development of 4.0 projects through the support of highly qualified managers • Orientation towards the innovation ecosystem: national and European competence centres (in particular the Smact Competence Centre in Triveneto), smart factories and demo centres, lighthouse factories, universities, technology clusters, public and private research centres, technology transfer centres, incubators and fablabs; • Support in accessing regional, national and European funding • Liaison with major regional clusters. SIAV is part of 12 technology clusters recognised by the Veneto Region. The DIH Veneto operates at a regional level in close connection with the "territorial antennas" set up by the Industrial Associations of the Veneto provinces and the provincial DIHs of Confindustria. Confindustria Veneto and SIAV participate in EEN - Enterprise Europe Network in the Friend Europe Consortium, pursuing the mission of internationalisation of enterprises in connection with territorial associations. SIAV participates in two EDIHs: DANTE - Digital Solutions for a Healthy, Active and Smart Life and NEURAL - Veneto Hub for Advanced Digital Technologies. In both EDIH, our core activity is animation of the industrial ecosystem (SMEs/regional clusters) and the provision of assessments on the digital maturity of enterprises, in particular manufacturing SMEs. As SIAV, we are also an observatory for the Veneto region on industrial transformations, we have also conducted research on industrial transitions in manufacturing SMEs and we carried out initiatives, projects, piloting and training activities with and within SMEs on both knowledge and technology transfer. Liaison with major regional clusters: SIAV is part of 12 technology clusters recognised by the Veneto Region (RIR- Reti Innovative Regionali)</t>
@@ -13258,16 +12845,14 @@
       </c>
     </row>
     <row r="211">
-      <c r="A211" s="1" t="inlineStr">
+      <c r="A211" s="1" t="n">
+        <v>209</v>
+      </c>
+      <c r="B211" t="inlineStr">
         <is>
           <t>ECIPA</t>
         </is>
       </c>
-      <c r="B211" t="inlineStr">
-        <is>
-          <t>ECIPA</t>
-        </is>
-      </c>
       <c r="C211" t="inlineStr">
         <is>
           <t>Ecipa developed the following offer of services, which are delivered by the DIH: Orientation activities in the form of awareness-raising workshops about the potential of digital transformation; Assessment of company maturity vis à vis Industry 4.0; Demonstration activities to approach digital technologies practically (e.g. prototyping); Training for SMEs willing to approach digital transformation; Support to the drafting of feasibility analysis of digital transformation processes; Support to the elaboration of digital transformation strategy; Consulting services on how to introduce digital optimisation or innovation; Support for identification of and access to funding opportunities for digital innovation; Networking among relevant stakeholders; Support for scaling up digital transformation with the help of Competence Centers. In 2017, CNA Veneto nominated Ecipa as the organization tasked with the development and management of the Digital Innovation Hub (DIH)</t>
@@ -13315,16 +12900,14 @@
       </c>
     </row>
     <row r="212">
-      <c r="A212" s="1" t="inlineStr">
+      <c r="A212" s="1" t="n">
+        <v>210</v>
+      </c>
+      <c r="B212" t="inlineStr">
         <is>
           <t>Flanders Make</t>
         </is>
       </c>
-      <c r="B212" t="inlineStr">
-        <is>
-          <t>Flanders Make</t>
-        </is>
-      </c>
       <c r="C212" t="inlineStr">
         <is>
           <t>The goal of DIGITALIS partners is to primarily help Flemish end user manufacturing SMEs in their digital and green transition. Although the prime focus is on SMEs we will also support bigger companies when applicable and especially when a connection can be made with an SME. Therefore our prime goals are: 1. Increase the uptake of digital technologies on the shopfloor of manufacturing SMEs 2. Increase the level of digital skills on the shopfloor 3. Play an active role in the European network of Digital Innovation Hubs 4. Actively contribute to the European Green Deal goals The partnership will work together in a lean governance model (see WP6) and provide a broad range of services: • Testing – manufacturing SMEs will be offered access to the DIGITALIS infrastructures to be able to test new digital shop floor technologies before implementing them – see WP2 • Providing training related to digital skills – DIGITALIS will train and upskill the workforce in manufacturing companies. To fully deploy the benefits of digitalisation different trainings will be offered for different levels in the organisation (shop floor people as well management, engineering, support) – see WP3 • Support to find the necessary financial means – we will help manufacturing SMEs to define the funds needed for the digital transition and in finding the most suitable financial means for the digital projects to fast-track the implementation at the SMEs – see WP4 • Ecosystem – we will enhance peer to peer learning both regional and on a European level and connect technology suppliers with end user SMEs to expand the digital ecosystem – see WP5 Participation in different living labs organized by our national funding agency. Act as technology service provider for the industry.</t>
@@ -13372,16 +12955,14 @@
       </c>
     </row>
     <row r="213">
-      <c r="A213" s="1" t="inlineStr">
+      <c r="A213" s="1" t="n">
+        <v>211</v>
+      </c>
+      <c r="B213" t="inlineStr">
         <is>
           <t>DIH4GlobalAutomotive</t>
         </is>
       </c>
-      <c r="B213" t="inlineStr">
-        <is>
-          <t>DIH4GlobalAutomotive</t>
-        </is>
-      </c>
       <c r="C213" t="inlineStr">
         <is>
           <t>The DIH 4 GLOBAL AUTOMOTIVE proposes to assume as the Digital Innovation Hub of the Automotive Sector in Portugal, arising from the aggregation of a set of entities and companies, coordinated by MOBINOV, with the objective of providing support services to SME to support the (necessary) digital transformation of the value chain, both at the product and process level, positioning existing companies and start-ups in the future of mobility. Its main objective is to work at the level of the development of innovative concepts and products for the Car of the Future, supporting the SMEs in the automotive sector in the development of new components for this car and, mainly, to support the necessary changes to the production processes associated with Industry 4.0 and the concept of Factory of the Future. It also intends to act as an access point to the European network of EDIHs, helping local companies and/or public actors to get support from other EDIHs in case the needed competences fall outside their competence, ensuring that every stakeholder gets the needed support wherever it is available in Europe and provide services to SME from other countries presented by other EDIHs that need their expertise. The diagnoses made with SMEs, point to the importance that digital technologies will be used increasingly in all car systems, so DIH resources will also be able to be mobilized in a transversal way, so that services can be provided with maximum flexibility and versatility. The DIH will act as an intermediary of innovation in the automotive industry and its value chain, seeking to provide through the provision of advanced digital services and technologies aid and support to companies in their digital transformation processes, providing a set of services such as testing before investing, skills development and training, support in the search for investment funding, partnerships and networking for the innovation ecosystem.</t>
@@ -13429,10 +13010,8 @@
       </c>
     </row>
     <row r="214">
-      <c r="A214" s="1" t="inlineStr">
-        <is>
-          <t>DInO</t>
-        </is>
+      <c r="A214" s="1" t="n">
+        <v>212</v>
       </c>
       <c r="B214" t="inlineStr">
         <is>
@@ -13482,10 +13061,8 @@
       </c>
     </row>
     <row r="215">
-      <c r="A215" s="1" t="inlineStr">
-        <is>
-          <t>AI EDIH Hungary</t>
-        </is>
+      <c r="A215" s="1" t="n">
+        <v>213</v>
       </c>
       <c r="B215" t="inlineStr">
         <is>
@@ -13539,10 +13116,8 @@
       </c>
     </row>
     <row r="216">
-      <c r="A216" s="1" t="inlineStr">
-        <is>
-          <t>DIBI</t>
-        </is>
+      <c r="A216" s="1" t="n">
+        <v>214</v>
       </c>
       <c r="B216" t="inlineStr">
         <is>
@@ -13596,10 +13171,8 @@
       </c>
     </row>
     <row r="217">
-      <c r="A217" s="1" t="inlineStr">
-        <is>
-          <t>EDIH DIGICARE</t>
-        </is>
+      <c r="A217" s="1" t="n">
+        <v>215</v>
       </c>
       <c r="B217" t="inlineStr">
         <is>
@@ -13649,10 +13222,8 @@
       </c>
     </row>
     <row r="218">
-      <c r="A218" s="1" t="inlineStr">
-        <is>
-          <t>EDIH NEB</t>
-        </is>
+      <c r="A218" s="1" t="n">
+        <v>216</v>
       </c>
       <c r="B218" t="inlineStr">
         <is>
@@ -13706,10 +13277,8 @@
       </c>
     </row>
     <row r="219">
-      <c r="A219" s="1" t="inlineStr">
-        <is>
-          <t>HPC EDIH HU</t>
-        </is>
+      <c r="A219" s="1" t="n">
+        <v>217</v>
       </c>
       <c r="B219" t="inlineStr">
         <is>
@@ -13770,10 +13339,8 @@
       </c>
     </row>
     <row r="220">
-      <c r="A220" s="1" t="inlineStr">
-        <is>
-          <t>Applied CPS</t>
-        </is>
+      <c r="A220" s="1" t="n">
+        <v>218</v>
       </c>
       <c r="B220" t="inlineStr">
         <is>
@@ -13829,10 +13396,8 @@
       </c>
     </row>
     <row r="221">
-      <c r="A221" s="1" t="inlineStr">
-        <is>
-          <t>DEDIHCATED BFC</t>
-        </is>
+      <c r="A221" s="1" t="n">
+        <v>219</v>
       </c>
       <c r="B221" t="inlineStr">
         <is>
@@ -13892,10 +13457,8 @@
       </c>
     </row>
     <row r="222">
-      <c r="A222" s="1" t="inlineStr">
-        <is>
-          <t>DIH4AISec</t>
-        </is>
+      <c r="A222" s="1" t="n">
+        <v>220</v>
       </c>
       <c r="B222" t="inlineStr">
         <is>
@@ -13949,10 +13512,8 @@
       </c>
     </row>
     <row r="223">
-      <c r="A223" s="1" t="inlineStr">
-        <is>
-          <t>MIDAS</t>
-        </is>
+      <c r="A223" s="1" t="n">
+        <v>221</v>
       </c>
       <c r="B223" t="inlineStr">
         <is>
@@ -14020,10 +13581,8 @@
       </c>
     </row>
     <row r="224">
-      <c r="A224" s="1" t="inlineStr">
-        <is>
-          <t>re_d</t>
-        </is>
+      <c r="A224" s="1" t="n">
+        <v>222</v>
       </c>
       <c r="B224" t="inlineStr">
         <is>
@@ -14077,10 +13636,8 @@
       </c>
     </row>
     <row r="225">
-      <c r="A225" s="1" t="inlineStr">
-        <is>
-          <t>EDIH-NWNL</t>
-        </is>
+      <c r="A225" s="1" t="n">
+        <v>223</v>
       </c>
       <c r="B225" t="inlineStr">
         <is>
@@ -14137,10 +13694,8 @@
       </c>
     </row>
     <row r="226">
-      <c r="A226" s="1" t="inlineStr">
-        <is>
-          <t>SynGReDiT</t>
-        </is>
+      <c r="A226" s="1" t="n">
+        <v>224</v>
       </c>
       <c r="B226" t="inlineStr">
         <is>
@@ -14194,10 +13749,8 @@
       </c>
     </row>
     <row r="227">
-      <c r="A227" s="1" t="inlineStr">
-        <is>
-          <t>EDIH Digital Trust</t>
-        </is>
+      <c r="A227" s="1" t="n">
+        <v>225</v>
       </c>
       <c r="B227" t="inlineStr">
         <is>
@@ -14251,10 +13804,8 @@
       </c>
     </row>
     <row r="228">
-      <c r="A228" s="1" t="inlineStr">
-        <is>
-          <t>EDIH-AICS</t>
-        </is>
+      <c r="A228" s="1" t="n">
+        <v>226</v>
       </c>
       <c r="B228" t="inlineStr">
         <is>
@@ -14308,10 +13859,8 @@
       </c>
     </row>
     <row r="229">
-      <c r="A229" s="1" t="inlineStr">
-        <is>
-          <t>HD-MOTION</t>
-        </is>
+      <c r="A229" s="1" t="n">
+        <v>227</v>
       </c>
       <c r="B229" t="inlineStr">
         <is>
@@ -14361,10 +13910,8 @@
       </c>
     </row>
     <row r="230">
-      <c r="A230" s="1" t="inlineStr">
-        <is>
-          <t>P.R.I.D.E.</t>
-        </is>
+      <c r="A230" s="1" t="n">
+        <v>228</v>
       </c>
       <c r="B230" t="inlineStr">
         <is>
@@ -14414,10 +13961,8 @@
       </c>
     </row>
     <row r="231">
-      <c r="A231" s="1" t="inlineStr">
-        <is>
-          <t>DIH4CN</t>
-        </is>
+      <c r="A231" s="1" t="n">
+        <v>229</v>
       </c>
       <c r="B231" t="inlineStr">
         <is>
@@ -14471,10 +14016,8 @@
       </c>
     </row>
     <row r="232">
-      <c r="A232" s="1" t="inlineStr">
-        <is>
-          <t>DIHNAMO</t>
-        </is>
+      <c r="A232" s="1" t="n">
+        <v>230</v>
       </c>
       <c r="B232" t="inlineStr">
         <is>
@@ -14520,10 +14063,8 @@
       </c>
     </row>
     <row r="233">
-      <c r="A233" s="1" t="inlineStr">
-        <is>
-          <t>DMH</t>
-        </is>
+      <c r="A233" s="1" t="n">
+        <v>231</v>
       </c>
       <c r="B233" t="inlineStr">
         <is>
@@ -14573,10 +14114,8 @@
       </c>
     </row>
     <row r="234">
-      <c r="A234" s="1" t="inlineStr">
-        <is>
-          <t>PBDH</t>
-        </is>
+      <c r="A234" s="1" t="n">
+        <v>232</v>
       </c>
       <c r="B234" t="inlineStr">
         <is>
@@ -14635,10 +14174,8 @@
       <c r="K234" t="inlineStr"/>
     </row>
     <row r="235">
-      <c r="A235" s="1" t="inlineStr">
-        <is>
-          <t>Data-EDIH</t>
-        </is>
+      <c r="A235" s="1" t="n">
+        <v>233</v>
       </c>
       <c r="B235" t="inlineStr">
         <is>
@@ -14694,10 +14231,8 @@
       </c>
     </row>
     <row r="236">
-      <c r="A236" s="1" t="inlineStr">
-        <is>
-          <t>EDIH Corsica.ai</t>
-        </is>
+      <c r="A236" s="1" t="n">
+        <v>234</v>
       </c>
       <c r="B236" t="inlineStr">
         <is>
@@ -14751,10 +14286,8 @@
       </c>
     </row>
     <row r="237">
-      <c r="A237" s="1" t="inlineStr">
-        <is>
-          <t>EDIH-SH</t>
-        </is>
+      <c r="A237" s="1" t="n">
+        <v>235</v>
       </c>
       <c r="B237" t="inlineStr">
         <is>
@@ -14808,10 +14341,8 @@
       </c>
     </row>
     <row r="238">
-      <c r="A238" s="1" t="inlineStr">
-        <is>
-          <t>Health Data Sweden (HDS)</t>
-        </is>
+      <c r="A238" s="1" t="n">
+        <v>236</v>
       </c>
       <c r="B238" t="inlineStr">
         <is>
@@ -14861,10 +14392,8 @@
       </c>
     </row>
     <row r="239">
-      <c r="A239" s="1" t="inlineStr">
-        <is>
-          <t>HEALTH HUB</t>
-        </is>
+      <c r="A239" s="1" t="n">
+        <v>237</v>
       </c>
       <c r="B239" t="inlineStr">
         <is>
@@ -14919,10 +14448,8 @@
       </c>
     </row>
     <row r="240">
-      <c r="A240" s="1" t="inlineStr">
-        <is>
-          <t>HHFIN</t>
-        </is>
+      <c r="A240" s="1" t="n">
+        <v>238</v>
       </c>
       <c r="B240" t="inlineStr">
         <is>
@@ -14974,10 +14501,8 @@
       </c>
     </row>
     <row r="241">
-      <c r="A241" s="1" t="inlineStr">
-        <is>
-          <t>eDIH-DIZ</t>
-        </is>
+      <c r="A241" s="1" t="n">
+        <v>239</v>
       </c>
       <c r="B241" t="inlineStr">
         <is>
@@ -15031,10 +14556,8 @@
       </c>
     </row>
     <row r="242">
-      <c r="A242" s="1" t="inlineStr">
-        <is>
-          <t>AI4HEALTH.Cro</t>
-        </is>
+      <c r="A242" s="1" t="n">
+        <v>240</v>
       </c>
       <c r="B242" t="inlineStr">
         <is>
@@ -15088,10 +14611,8 @@
       </c>
     </row>
     <row r="243">
-      <c r="A243" s="1" t="inlineStr">
-        <is>
-          <t>smartHEALTH</t>
-        </is>
+      <c r="A243" s="1" t="n">
+        <v>241</v>
       </c>
       <c r="B243" t="inlineStr">
         <is>
@@ -15145,10 +14666,8 @@
       </c>
     </row>
     <row r="244">
-      <c r="A244" s="1" t="inlineStr">
-        <is>
-          <t>DigiHealthPT</t>
-        </is>
+      <c r="A244" s="1" t="n">
+        <v>242</v>
       </c>
       <c r="B244" t="inlineStr">
         <is>
@@ -15198,10 +14717,8 @@
       </c>
     </row>
     <row r="245">
-      <c r="A245" s="1" t="inlineStr">
-        <is>
-          <t>CiTyInnoHub</t>
-        </is>
+      <c r="A245" s="1" t="n">
+        <v>243</v>
       </c>
       <c r="B245" t="inlineStr">
         <is>
@@ -15251,10 +14768,8 @@
       </c>
     </row>
     <row r="246">
-      <c r="A246" s="1" t="inlineStr">
-        <is>
-          <t>DANTE</t>
-        </is>
+      <c r="A246" s="1" t="n">
+        <v>244</v>
       </c>
       <c r="B246" t="inlineStr">
         <is>
@@ -15308,10 +14823,8 @@
       </c>
     </row>
     <row r="247">
-      <c r="A247" s="1" t="inlineStr">
-        <is>
-          <t>DigIT Hub Sweden</t>
-        </is>
+      <c r="A247" s="1" t="n">
+        <v>245</v>
       </c>
       <c r="B247" t="inlineStr">
         <is>
@@ -15366,10 +14879,8 @@
       </c>
     </row>
     <row r="248">
-      <c r="A248" s="1" t="inlineStr">
-        <is>
-          <t>EDIH4DT</t>
-        </is>
+      <c r="A248" s="1" t="n">
+        <v>246</v>
       </c>
       <c r="B248" t="inlineStr">
         <is>
@@ -15423,10 +14934,8 @@
       </c>
     </row>
     <row r="249">
-      <c r="A249" s="1" t="inlineStr">
-        <is>
-          <t>EDITH</t>
-        </is>
+      <c r="A249" s="1" t="n">
+        <v>247</v>
       </c>
       <c r="B249" t="inlineStr">
         <is>
@@ -15480,10 +14989,8 @@
       </c>
     </row>
     <row r="250">
-      <c r="A250" s="1" t="inlineStr">
-        <is>
-          <t>GR digiGOV-innoHUB</t>
-        </is>
+      <c r="A250" s="1" t="n">
+        <v>248</v>
       </c>
       <c r="B250" t="inlineStr">
         <is>
@@ -15538,10 +15045,8 @@
       </c>
     </row>
     <row r="251">
-      <c r="A251" s="1" t="inlineStr">
-        <is>
-          <t>I-NEST</t>
-        </is>
+      <c r="A251" s="1" t="n">
+        <v>249</v>
       </c>
       <c r="B251" t="inlineStr">
         <is>
@@ -15595,10 +15100,8 @@
       </c>
     </row>
     <row r="252">
-      <c r="A252" s="1" t="inlineStr">
-        <is>
-          <t>MDZ Franken</t>
-        </is>
+      <c r="A252" s="1" t="n">
+        <v>250</v>
       </c>
       <c r="B252" t="inlineStr">
         <is>
@@ -15652,10 +15155,8 @@
       </c>
     </row>
     <row r="253">
-      <c r="A253" s="1" t="inlineStr">
-        <is>
-          <t>VNG NL DIGI HUB</t>
-        </is>
+      <c r="A253" s="1" t="n">
+        <v>251</v>
       </c>
       <c r="B253" t="inlineStr">
         <is>
@@ -15724,10 +15225,8 @@
       </c>
     </row>
     <row r="254">
-      <c r="A254" s="1" t="inlineStr">
-        <is>
-          <t>AI4PA_Portugal</t>
-        </is>
+      <c r="A254" s="1" t="n">
+        <v>252</v>
       </c>
       <c r="B254" t="inlineStr">
         <is>
@@ -15781,10 +15280,8 @@
       </c>
     </row>
     <row r="255">
-      <c r="A255" s="1" t="inlineStr">
-        <is>
-          <t>EDIH Thuringia</t>
-        </is>
+      <c r="A255" s="1" t="n">
+        <v>253</v>
       </c>
       <c r="B255" t="inlineStr">
         <is>
@@ -15834,10 +15331,8 @@
       </c>
     </row>
     <row r="256">
-      <c r="A256" s="1" t="inlineStr">
-        <is>
-          <t>Aragon EDIH</t>
-        </is>
+      <c r="A256" s="1" t="n">
+        <v>254</v>
       </c>
       <c r="B256" t="inlineStr">
         <is>
@@ -15891,10 +15386,8 @@
       </c>
     </row>
     <row r="257">
-      <c r="A257" s="1" t="inlineStr">
-        <is>
-          <t>EasyHPC</t>
-        </is>
+      <c r="A257" s="1" t="n">
+        <v>255</v>
       </c>
       <c r="B257" t="inlineStr">
         <is>
@@ -15951,10 +15444,8 @@
       </c>
     </row>
     <row r="258">
-      <c r="A258" s="1" t="inlineStr">
-        <is>
-          <t>UDIH 4 EU</t>
-        </is>
+      <c r="A258" s="1" t="n">
+        <v>256</v>
       </c>
       <c r="B258" t="inlineStr">
         <is>
@@ -16008,10 +15499,8 @@
       </c>
     </row>
     <row r="259">
-      <c r="A259" s="1" t="inlineStr">
-        <is>
-          <t>AEDIH</t>
-        </is>
+      <c r="A259" s="1" t="n">
+        <v>257</v>
       </c>
       <c r="B259" t="inlineStr">
         <is>
@@ -16061,10 +15550,8 @@
       </c>
     </row>
     <row r="260">
-      <c r="A260" s="1" t="inlineStr">
-        <is>
-          <t>GC EDIH</t>
-        </is>
+      <c r="A260" s="1" t="n">
+        <v>258</v>
       </c>
       <c r="B260" t="inlineStr">
         <is>
@@ -16119,10 +15606,8 @@
       </c>
     </row>
     <row r="261">
-      <c r="A261" s="1" t="inlineStr">
-        <is>
-          <t>HPC4Poland EDIH</t>
-        </is>
+      <c r="A261" s="1" t="n">
+        <v>259</v>
       </c>
       <c r="B261" t="inlineStr">
         <is>
@@ -16176,10 +15661,8 @@
       </c>
     </row>
     <row r="262">
-      <c r="A262" s="1" t="inlineStr">
-        <is>
-          <t>EDIH West Marmara</t>
-        </is>
+      <c r="A262" s="1" t="n">
+        <v>260</v>
       </c>
       <c r="B262" t="inlineStr">
         <is>
@@ -16233,10 +15716,8 @@
       </c>
     </row>
     <row r="263">
-      <c r="A263" s="1" t="inlineStr">
-        <is>
-          <t>S4AI_HUB</t>
-        </is>
+      <c r="A263" s="1" t="n">
+        <v>261</v>
       </c>
       <c r="B263" t="inlineStr">
         <is>
@@ -16292,10 +15773,8 @@
       </c>
     </row>
     <row r="264">
-      <c r="A264" s="1" t="inlineStr">
-        <is>
-          <t>DIVA</t>
-        </is>
+      <c r="A264" s="1" t="n">
+        <v>262</v>
       </c>
       <c r="B264" t="inlineStr">
         <is>
@@ -16349,10 +15828,8 @@
       </c>
     </row>
     <row r="265">
-      <c r="A265" s="1" t="inlineStr">
-        <is>
-          <t>ZP EDIH</t>
-        </is>
+      <c r="A265" s="1" t="n">
+        <v>263</v>
       </c>
       <c r="B265" t="inlineStr">
         <is>
@@ -16406,10 +15883,8 @@
       </c>
     </row>
     <row r="266">
-      <c r="A266" s="1" t="inlineStr">
-        <is>
-          <t>Eastern Ukraine EDIH</t>
-        </is>
+      <c r="A266" s="1" t="n">
+        <v>264</v>
       </c>
       <c r="B266" t="inlineStr">
         <is>
@@ -16465,10 +15940,8 @@
       </c>
     </row>
     <row r="267">
-      <c r="A267" s="1" t="inlineStr">
-        <is>
-          <t>EDIH B4I</t>
-        </is>
+      <c r="A267" s="1" t="n">
+        <v>265</v>
       </c>
       <c r="B267" t="inlineStr">
         <is>
@@ -16522,16 +15995,14 @@
       </c>
     </row>
     <row r="268">
-      <c r="A268" s="1" t="inlineStr">
+      <c r="A268" s="1" t="n">
+        <v>266</v>
+      </c>
+      <c r="B268" t="inlineStr">
         <is>
           <t>EUNITED Digital Hub</t>
         </is>
       </c>
-      <c r="B268" t="inlineStr">
-        <is>
-          <t>EUNITED Digital Hub</t>
-        </is>
-      </c>
       <c r="C268" t="inlineStr">
         <is>
           <t>EUNITED Digital Hub is a European Digital Innovation Hub (EDIH) led by UNIT.City, Ukraine’s largest innovation park, in partnership with 16 partners: universities, NGOs, and industry leaders. It is not just a service provider — it is an ecosystem builder. EUNITED is a powerful consortium fostering collaboration, innovation, and resilience for SMEs and public institutions supporting the movement towards a stronger, smarter, and globally competitive Ukraine as a part of the European family.</t>
@@ -16579,10 +16050,8 @@
       </c>
     </row>
     <row r="269">
-      <c r="A269" s="1" t="inlineStr">
-        <is>
-          <t>Digitalzh</t>
-        </is>
+      <c r="A269" s="1" t="n">
+        <v>267</v>
       </c>
       <c r="B269" t="inlineStr">
         <is>
@@ -16636,10 +16105,8 @@
       </c>
     </row>
     <row r="270">
-      <c r="A270" s="1" t="inlineStr">
-        <is>
-          <t>EDIH4UrbanSAVE</t>
-        </is>
+      <c r="A270" s="1" t="n">
+        <v>268</v>
       </c>
       <c r="B270" t="inlineStr">
         <is>
@@ -16693,16 +16160,14 @@
       </c>
     </row>
     <row r="271">
-      <c r="A271" s="1" t="inlineStr">
+      <c r="A271" s="1" t="n">
+        <v>269</v>
+      </c>
+      <c r="B271" t="inlineStr">
         <is>
           <t>INFAB HUB</t>
         </is>
       </c>
-      <c r="B271" t="inlineStr">
-        <is>
-          <t>INFAB HUB</t>
-        </is>
-      </c>
       <c r="C271" t="inlineStr">
         <is>
           <t>The INFAB HUB has as its priority objectives the promotion and development of innovation in the business fabric in order to achieve a higher level of competitiveness and the promotion of an appropriate legal framework for the development of this industry and its promotion within and outside the autonomous region. In the same way, it works actively to achieve common objectives in the field of innovative industrial activity, particularly in the development of projects that contribute to the creation, accumulation and dissemination of knowledge; in the improvement of productivity through greater innovation and process optimization among the activities of its members; in innovation, through joint research; and in the promotion of visibility, the strategic importance of industrial activity. HUB focuses on the digitalization of industry and related services for more efficient manufacturing processes. To achieve this, the HUB makes use of technologies such as blockchain, digital twin, internet of things, machine learning and also one of the key disruptive technologies in industry: Artificial Intelligence (AI), framed within the European Strategy for Artificial Intelligence (AI), as well as the Spanish Strategy for R&amp;D&amp;I in Artificial Intelligence, where the national priorities regarding Artificial Intelligence for the Spanish Strategy for Science, Technology and Innovation (EECTI) 2021-2028 are stated. Therefore, INFABHUB offers its expertise in the field to other companies to carry out a knowledge transfer to them, providing them with critical digital skills in order to achieve better productive manufacturing processes.</t>
@@ -16750,10 +16215,8 @@
       </c>
     </row>
     <row r="272">
-      <c r="A272" s="1" t="inlineStr">
-        <is>
-          <t>Move2Digital</t>
-        </is>
+      <c r="A272" s="1" t="n">
+        <v>270</v>
       </c>
       <c r="B272" t="inlineStr">
         <is>
@@ -16811,10 +16274,8 @@
       </c>
     </row>
     <row r="273">
-      <c r="A273" s="1" t="inlineStr">
-        <is>
-          <t>PICS2</t>
-        </is>
+      <c r="A273" s="1" t="n">
+        <v>271</v>
       </c>
       <c r="B273" t="inlineStr">
         <is>
@@ -16864,10 +16325,8 @@
       </c>
     </row>
     <row r="274">
-      <c r="A274" s="1" t="inlineStr">
-        <is>
-          <t>R.O.M.E. Digital Hub</t>
-        </is>
+      <c r="A274" s="1" t="n">
+        <v>272</v>
       </c>
       <c r="B274" t="inlineStr">
         <is>
@@ -16917,10 +16376,8 @@
       </c>
     </row>
     <row r="275">
-      <c r="A275" s="1" t="inlineStr">
-        <is>
-          <t>sustAIn.brussels</t>
-        </is>
+      <c r="A275" s="1" t="n">
+        <v>273</v>
       </c>
       <c r="B275" t="inlineStr">
         <is>
@@ -16974,10 +16431,8 @@
       </c>
     </row>
     <row r="276">
-      <c r="A276" s="1" t="inlineStr">
-        <is>
-          <t>Foundation for innovation and technology development, INTERA Technology Park</t>
-        </is>
+      <c r="A276" s="1" t="n">
+        <v>274</v>
       </c>
       <c r="B276" t="inlineStr">
         <is>
@@ -17027,10 +16482,8 @@
       </c>
     </row>
     <row r="277">
-      <c r="A277" s="1" t="inlineStr">
-        <is>
-          <t>Cineca</t>
-        </is>
+      <c r="A277" s="1" t="n">
+        <v>275</v>
       </c>
       <c r="B277" t="inlineStr">
         <is>
@@ -17084,10 +16537,8 @@
       </c>
     </row>
     <row r="278">
-      <c r="A278" s="1" t="inlineStr">
-        <is>
-          <t>CNA HUB 4.0</t>
-        </is>
+      <c r="A278" s="1" t="n">
+        <v>276</v>
       </c>
       <c r="B278" t="inlineStr">
         <is>
@@ -17152,10 +16603,8 @@
       </c>
     </row>
     <row r="279">
-      <c r="A279" s="1" t="inlineStr">
-        <is>
-          <t>HUB4.0MANUVAL</t>
-        </is>
+      <c r="A279" s="1" t="n">
+        <v>277</v>
       </c>
       <c r="B279" t="inlineStr">
         <is>
@@ -17209,10 +16658,8 @@
       </c>
     </row>
     <row r="280">
-      <c r="A280" s="1" t="inlineStr">
-        <is>
-          <t>ICD</t>
-        </is>
+      <c r="A280" s="1" t="n">
+        <v>278</v>
       </c>
       <c r="B280" t="inlineStr">
         <is>
@@ -17266,10 +16713,8 @@
       </c>
     </row>
     <row r="281">
-      <c r="A281" s="1" t="inlineStr">
-        <is>
-          <t>JSI</t>
-        </is>
+      <c r="A281" s="1" t="n">
+        <v>279</v>
       </c>
       <c r="B281" t="inlineStr">
         <is>
@@ -17323,10 +16768,8 @@
       </c>
     </row>
     <row r="282">
-      <c r="A282" s="1" t="inlineStr">
-        <is>
-          <t>SINTEF</t>
-        </is>
+      <c r="A282" s="1" t="n">
+        <v>280</v>
       </c>
       <c r="B282" t="inlineStr">
         <is>
@@ -17380,10 +16823,8 @@
       </c>
     </row>
     <row r="283">
-      <c r="A283" s="1" t="inlineStr">
-        <is>
-          <t>CyberDIH</t>
-        </is>
+      <c r="A283" s="1" t="n">
+        <v>281</v>
       </c>
       <c r="B283" t="inlineStr">
         <is>
@@ -17437,10 +16878,8 @@
       </c>
     </row>
     <row r="284">
-      <c r="A284" s="1" t="inlineStr">
-        <is>
-          <t>DIGIHALL</t>
-        </is>
+      <c r="A284" s="1" t="n">
+        <v>282</v>
       </c>
       <c r="B284" t="inlineStr">
         <is>
@@ -17494,10 +16933,8 @@
       </c>
     </row>
     <row r="285">
-      <c r="A285" s="1" t="inlineStr">
-        <is>
-          <t>ATTRACT</t>
-        </is>
+      <c r="A285" s="1" t="n">
+        <v>283</v>
       </c>
       <c r="B285" t="inlineStr">
         <is>
@@ -17554,10 +16991,8 @@
       </c>
     </row>
     <row r="286">
-      <c r="A286" s="1" t="inlineStr">
-        <is>
-          <t>EDIH LA REUNION</t>
-        </is>
+      <c r="A286" s="1" t="n">
+        <v>284</v>
       </c>
       <c r="B286" t="inlineStr">
         <is>
@@ -17607,10 +17042,8 @@
       </c>
     </row>
     <row r="287">
-      <c r="A287" s="1" t="inlineStr">
-        <is>
-          <t>LVDH</t>
-        </is>
+      <c r="A287" s="1" t="n">
+        <v>285</v>
       </c>
       <c r="B287" t="inlineStr">
         <is>
@@ -17660,10 +17093,8 @@
       </c>
     </row>
     <row r="288">
-      <c r="A288" s="1" t="inlineStr">
-        <is>
-          <t>Ap-EDIH</t>
-        </is>
+      <c r="A288" s="1" t="n">
+        <v>286</v>
       </c>
       <c r="B288" t="inlineStr">
         <is>
@@ -17713,10 +17144,8 @@
       </c>
     </row>
     <row r="289">
-      <c r="A289" s="1" t="inlineStr">
-        <is>
-          <t>CyberSec</t>
-        </is>
+      <c r="A289" s="1" t="n">
+        <v>287</v>
       </c>
       <c r="B289" t="inlineStr">
         <is>
@@ -17770,10 +17199,8 @@
       </c>
     </row>
     <row r="290">
-      <c r="A290" s="1" t="inlineStr">
-        <is>
-          <t>DAMAS</t>
-        </is>
+      <c r="A290" s="1" t="n">
+        <v>288</v>
       </c>
       <c r="B290" t="inlineStr">
         <is>
@@ -17827,10 +17254,8 @@
       </c>
     </row>
     <row r="291">
-      <c r="A291" s="1" t="inlineStr">
-        <is>
-          <t>POLIDIH</t>
-        </is>
+      <c r="A291" s="1" t="n">
+        <v>289</v>
       </c>
       <c r="B291" t="inlineStr">
         <is>
@@ -17886,10 +17311,8 @@
       </c>
     </row>
     <row r="292">
-      <c r="A292" s="1" t="inlineStr">
-        <is>
-          <t>Digital Impact North (DIN)</t>
-        </is>
+      <c r="A292" s="1" t="n">
+        <v>290</v>
       </c>
       <c r="B292" t="inlineStr">
         <is>
@@ -17943,10 +17366,8 @@
       </c>
     </row>
     <row r="293">
-      <c r="A293" s="1" t="inlineStr">
-        <is>
-          <t>LEAP EDIH</t>
-        </is>
+      <c r="A293" s="1" t="n">
+        <v>291</v>
       </c>
       <c r="B293" t="inlineStr">
         <is>
@@ -18002,10 +17423,8 @@
       </c>
     </row>
     <row r="294">
-      <c r="A294" s="1" t="inlineStr">
-        <is>
-          <t>EDIH Adria</t>
-        </is>
+      <c r="A294" s="1" t="n">
+        <v>292</v>
       </c>
       <c r="B294" t="inlineStr">
         <is>
@@ -18066,10 +17485,8 @@
       </c>
     </row>
     <row r="295">
-      <c r="A295" s="1" t="inlineStr">
-        <is>
-          <t>Malta-EDIH</t>
-        </is>
+      <c r="A295" s="1" t="n">
+        <v>293</v>
       </c>
       <c r="B295" t="inlineStr">
         <is>
@@ -18124,10 +17541,8 @@
       </c>
     </row>
     <row r="296">
-      <c r="A296" s="1" t="inlineStr">
-        <is>
-          <t>OCEANOPOLIS</t>
-        </is>
+      <c r="A296" s="1" t="n">
+        <v>294</v>
       </c>
       <c r="B296" t="inlineStr">
         <is>
@@ -18205,16 +17620,14 @@
       </c>
     </row>
     <row r="297">
-      <c r="A297" s="1" t="inlineStr">
+      <c r="A297" s="1" t="n">
+        <v>295</v>
+      </c>
+      <c r="B297" t="inlineStr">
         <is>
           <t>Mittelstand-Digital Zentrum Lingen.Münster.Osnarbrück</t>
         </is>
       </c>
-      <c r="B297" t="inlineStr">
-        <is>
-          <t>Mittelstand-Digital Zentrum Lingen.Münster.Osnarbrück</t>
-        </is>
-      </c>
       <c r="C297" t="inlineStr">
         <is>
           <t>Our mission: to digitize the SME sector! Because we believe that the digital transformation brings new opportunities - and we want to make these available to everyone! The digital transformation is changing the world of work in many ways. New business models and competitive structures are emerging. Innovative technologies and the use of data are creating additional opportunities. Digitalization should simplify and optimize processes, relieve employees, enable flexibility and make your company fit for the future in the long term. The Mittelstand-Digital Zentrum Lingen.Münster.Osnabrück therefore accompanies small and medium-sized enterprises (SMEs) on their path to digital transformation and supports them in the design and implementation of sustainable business models.</t>
@@ -18262,10 +17675,8 @@
       </c>
     </row>
     <row r="298">
-      <c r="A298" s="1" t="inlineStr">
-        <is>
-          <t>FTCH</t>
-        </is>
+      <c r="A298" s="1" t="n">
+        <v>296</v>
       </c>
       <c r="B298" t="inlineStr">
         <is>
@@ -18332,6 +17743,53 @@
       <c r="K298" t="inlineStr">
         <is>
           <t>Artificial Intelligence &amp; Decision support - 5, Big data - 4, Blockchain and Distributed Ledger Technology (DLT) - 4, Cybersecurity - 4, Logistics - 1, Cloud Services - 4, Internet of Things - 2, Internet Services &amp; Applications - 3, Virtual Reality - 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" s="1" t="n">
+        <v>297</v>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>AI and Robotics Estonia (EDIH)</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>The artificial intelligence (AI) and robotics EDIH AIRE facilitates innovation in Estonian manufacturing by bringing together the core competencies of universities, science parks and research centres in the fields of AI and robotics, and the SMEs in Estonia and Europe, working in close collaboration with other AI-related centres and initiatives in Estonia and Europe. The hub is run by a highly capable and experienced consortium led by the Tallinn University of Technology, and its partners are the University of Tartu, the Estonian University of Life Sciences, Tehnopol Science and Business Park, Tartu Science Park, and competence centre IMECC, supported by other key stakeholders as associate partners. AIRE’s objectives are (1) to increase the digital maturity of the manufacturing SMEs, (2) to increase investments into industrial digitalisation, (3) to create sustainable EDIH ecosystem in Estonia and involve relevant stakeholders from the EU, (4) to improve the target groups' skills and competences on AI and robotics, and (5) to increase market maturity and market creation potential of Estonian innovations. To achieve this, the focus is on the ‘test before invest’ activities (WP2), incl. digital maturity assessment and related individual consulting and roadmapping for clients, and implementation of proof-of-concept AI and robotics demo projects and experiments with manufacturing companies. This is supported by AI and robotics related trainings (WP3), access to finance services (WP4) and ecosystem development (WP5). AIRE will contribute to long-term policy objectives of Estonia and the EU. Based on the strategic view of the Estonian state, in 2022-2025 AIRE focuses on the manufacturing industry as the primary target group and up to 10% of the budget is allocated to cross-sectoral AI pilots in health technology and tourism to widen the impact and illustrate transferability. From 2025+, AIRE will more strongly address a wider range of sectors in the future from 2025+.</t>
+        </is>
+      </c>
+      <c r="D299" t="inlineStr">
+        <is>
+          <t>Estonia</t>
+        </is>
+      </c>
+      <c r="E299" t="inlineStr">
+        <is>
+          <t>Kirke Maar</t>
+        </is>
+      </c>
+      <c r="F299" t="inlineStr">
+        <is>
+          <t>Ehitajate tee 5, 19086 Tallinn Estonia, Estonia</t>
+        </is>
+      </c>
+      <c r="G299" t="inlineStr">
+        <is>
+          <t>EDIH</t>
+        </is>
+      </c>
+      <c r="H299" t="inlineStr">
+        <is>
+          <t>https://aire-edih.eu/</t>
+        </is>
+      </c>
+      <c r="I299" t="inlineStr"/>
+      <c r="J299" t="inlineStr"/>
+      <c r="K299" t="inlineStr">
+        <is>
+          <t>Artificial Intelligence &amp; Decision support - 5, Robotics - 5, Big data - 3, BI tools - 3, data - 5, Digital twins - 3, Cybersecurity - 3, Internet of Things - 3, Laser-based manufacturing and materials processing - 3, Logistics - 3, Sensors &amp; Vision Processing Systems - 3, Simulation engineering and modelling - 4, Mobility - 3, Virtual Reality - 3, Cloud Services - 3, Chemical engineering (plants, products) - 3, Cyber-physical systems - 3, High performance computing - 3, Software Architectures - 3, Human computer interaction - 5, Industrial biotechnology - 3, Communication network - 3, Organic and large area electronics - 3, Displays - 3</t>
         </is>
       </c>
     </row>
@@ -19661,7 +19119,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19670,11 +19128,6 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>EDIH Name</t>
-        </is>
-      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
           <t>EDIH Title</t>
@@ -19727,10 +19180,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Mittelstand-Digital Zentrum Berlin</t>
-        </is>
+      <c r="A2" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -19780,10 +19231,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Mittelstand-Digital Zentrum Handwerk</t>
-        </is>
+      <c r="A3" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -19833,10 +19282,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>CICERO DIH</t>
-        </is>
+      <c r="A4" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -19886,10 +19333,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>Idele</t>
-        </is>
+      <c r="A5" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -19939,10 +19384,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>C-Hub</t>
-        </is>
+      <c r="A6" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -19996,10 +19439,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>InnovationAmp</t>
-        </is>
+      <c r="A7" s="1" t="n">
+        <v>73</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -20049,10 +19490,8 @@
       <c r="K7" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>EDIH-IS</t>
-        </is>
+      <c r="A8" s="1" t="n">
+        <v>99</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -20102,10 +19541,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>DInO</t>
-        </is>
+      <c r="A9" s="1" t="n">
+        <v>212</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -20155,10 +19592,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>PBDH</t>
-        </is>
+      <c r="A10" s="1" t="n">
+        <v>232</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -20215,6 +19650,53 @@
         </is>
       </c>
       <c r="K10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>297</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>AI and Robotics Estonia (EDIH)</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>The artificial intelligence (AI) and robotics EDIH AIRE facilitates innovation in Estonian manufacturing by bringing together the core competencies of universities, science parks and research centres in the fields of AI and robotics, and the SMEs in Estonia and Europe, working in close collaboration with other AI-related centres and initiatives in Estonia and Europe. The hub is run by a highly capable and experienced consortium led by the Tallinn University of Technology, and its partners are the University of Tartu, the Estonian University of Life Sciences, Tehnopol Science and Business Park, Tartu Science Park, and competence centre IMECC, supported by other key stakeholders as associate partners. AIRE’s objectives are (1) to increase the digital maturity of the manufacturing SMEs, (2) to increase investments into industrial digitalisation, (3) to create sustainable EDIH ecosystem in Estonia and involve relevant stakeholders from the EU, (4) to improve the target groups' skills and competences on AI and robotics, and (5) to increase market maturity and market creation potential of Estonian innovations. To achieve this, the focus is on the ‘test before invest’ activities (WP2), incl. digital maturity assessment and related individual consulting and roadmapping for clients, and implementation of proof-of-concept AI and robotics demo projects and experiments with manufacturing companies. This is supported by AI and robotics related trainings (WP3), access to finance services (WP4) and ecosystem development (WP5). AIRE will contribute to long-term policy objectives of Estonia and the EU. Based on the strategic view of the Estonian state, in 2022-2025 AIRE focuses on the manufacturing industry as the primary target group and up to 10% of the budget is allocated to cross-sectoral AI pilots in health technology and tourism to widen the impact and illustrate transferability. From 2025+, AIRE will more strongly address a wider range of sectors in the future from 2025+.</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Estonia</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Kirke Maar</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Ehitajate tee 5, 19086 Tallinn Estonia, Estonia</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>EDIH</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>https://aire-edih.eu/</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Artificial Intelligence &amp; Decision support - 5, Robotics - 5, Big data - 3, BI tools - 3, data - 5, Digital twins - 3, Cybersecurity - 3, Internet of Things - 3, Laser-based manufacturing and materials processing - 3, Logistics - 3, Sensors &amp; Vision Processing Systems - 3, Simulation engineering and modelling - 4, Mobility - 3, Virtual Reality - 3, Cloud Services - 3, Chemical engineering (plants, products) - 3, Cyber-physical systems - 3, High performance computing - 3, Software Architectures - 3, Human computer interaction - 5, Industrial biotechnology - 3, Communication network - 3, Organic and large area electronics - 3, Displays - 3</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -20227,7 +19709,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20236,11 +19718,6 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>EDIH Name</t>
-        </is>
-      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Formatted services</t>
@@ -20258,10 +19735,8 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>Mittelstand-Digital Zentrum Berlin</t>
-        </is>
+      <c r="A2" s="1" t="n">
+        <v>0</v>
       </c>
       <c r="B2" t="b">
         <v>0</v>
@@ -20274,10 +19749,8 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Mittelstand-Digital Zentrum Handwerk</t>
-        </is>
+      <c r="A3" s="1" t="n">
+        <v>1</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
@@ -20290,10 +19763,8 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>CICERO DIH</t>
-        </is>
+      <c r="A4" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="B4" t="b">
         <v>0</v>
@@ -20306,10 +19777,8 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>Idele</t>
-        </is>
+      <c r="A5" s="1" t="n">
+        <v>3</v>
       </c>
       <c r="B5" t="b">
         <v>0</v>
@@ -20322,10 +19791,8 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>C-Hub</t>
-        </is>
+      <c r="A6" s="1" t="n">
+        <v>4</v>
       </c>
       <c r="B6" t="b">
         <v>0</v>
@@ -20338,10 +19805,8 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>InnovationAmp</t>
-        </is>
+      <c r="A7" s="1" t="n">
+        <v>73</v>
       </c>
       <c r="B7" t="b">
         <v>0</v>
@@ -20354,10 +19819,8 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>EDIH-IS</t>
-        </is>
+      <c r="A8" s="1" t="n">
+        <v>99</v>
       </c>
       <c r="B8" t="b">
         <v>1</v>
@@ -20370,10 +19833,8 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>DInO</t>
-        </is>
+      <c r="A9" s="1" t="n">
+        <v>212</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -20386,10 +19847,8 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>PBDH</t>
-        </is>
+      <c r="A10" s="1" t="n">
+        <v>232</v>
       </c>
       <c r="B10" t="b">
         <v>0</v>
@@ -20399,6 +19858,20 @@
       </c>
       <c r="D10" t="b">
         <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>297</v>
+      </c>
+      <c r="B11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>